<commit_message>
Update 3/4 bài tập Phần 1: Learning Meaning, Learning Card, Generate Flexible
</commit_message>
<xml_diff>
--- a/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
+++ b/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -51,6 +51,29 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -58,7 +81,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none">
         <fgColor/>
@@ -73,12 +96,45 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFD5F6F2"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFF5EB"/>
         <bgColor/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD5F6F2"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -104,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -112,6 +168,15 @@
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -441,15 +506,15 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="42"/>
     <col collapsed="false" customWidth="true" hidden="false" max="4" min="4" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="63"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="10" min="10" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="11" min="11" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="8" min="8" style="0" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="9" min="9" style="0" width="63"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="10" min="10" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="11" min="11" style="0" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" max="12" min="12" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="13" min="13" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="14" min="14" style="0" width="22"/>
@@ -458,57 +523,80 @@
     <col collapsed="false" customWidth="true" hidden="false" max="17" min="17" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="18" min="18" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="19" min="19" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="20" min="20" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="21" min="21" style="0" width="22"/>
   </cols>
   <sheetData>
-    <row customHeight="true" ht="41" r="1">
-      <c r="A1" s="2" t="str">
+    <row customHeight="true" ht="40" r="1">
+      <c r="A1" s="3" t="str">
         <v>Công việc</v>
       </c>
-      <c r="B1" s="2" t="str">
+      <c r="B1" s="3" t="str">
         <v>Input</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C1" s="3" t="str">
         <v>Output</v>
       </c>
-      <c r="D1" s="2" t="str">
+      <c r="D1" s="3" t="str">
         <v>Tham khảo</v>
       </c>
-      <c r="E1" s="2" t="str">
+      <c r="E1" s="3" t="str">
         <v>Prompt của a Hoàng</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="str">
+      <c r="F1" s="4"/>
+      <c r="G1" s="2" t="str">
+        <v>input raw - từ Excel</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <v>output raw - từ Excel</v>
+      </c>
+      <c r="I1" s="2" t="str">
         <v>prompt Cường</v>
       </c>
-      <c r="H1" s="1" t="str">
-        <v>user_input</v>
+      <c r="J1" s="2" t="str">
+        <v>user_input - THOẢI MÁI, KO CẦN THEO JSON</v>
       </c>
-      <c r="I1" s="1" t="str">
+      <c r="K1" s="2" t="str">
         <v>output</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="2">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+    </row>
+    <row customHeight="true" ht="113" r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="str">
+        <v>[
+    {
+        "question":"Which company are you working for?",
+        "structure":"I'm the ______ from ABC Company. ",
+        "main phrase":"Sales representative",
+        "optional phrase 1":"Sales director",
+        "optional phrase 2":"Sales associate"
+        "question-vi":"Bạn đang làm việc cho công ty nào vậy?",
+        "structure-vi":"Tôi là _____ từ công ty ABC.",
+        "main phrase-vi":"Đại diện kinh doanh",
+        "optional phrase 1-vi":"Giám đốc kinh doanh",
+        "optional phrase 2-vi":"Nhân viên bán hàng"
+    }
+]</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -517,19 +605,21 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="3">
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -538,8 +628,10 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-    </row>
-    <row customHeight="true" ht="146" r="4">
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="4">
       <c r="A4" s="1" t="str" xml:space="preserve">
         <v>Dạng 1: Learning Meaning Exercise </v>
       </c>
@@ -548,7 +640,38 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="str">
+      <c r="G4" s="5" t="str" xml:space="preserve">
+        <v>Câu hỏi
+Cấu trúc
+Cụm thông tin
+Main phrase
+Optional phrase
+Which company are you working for?
+I'm the ______ from ABC Company. 
+Sales representative
+Sales director
+Sales associate
+ </v>
+      </c>
+      <c r="H4" s="5" t="str" xml:space="preserve">
+        <v>description
+sentence
+answer_1
+answer_2
+answer_3
+Hãy dịch cụm in đậm
+I'm the &lt;g&gt;Đại diện kinh doanh&lt;/g&gt; from ABC Company.
+Sales representative
+Sales director
+Sales Associate
+Hãy dịch cụm in đậm
+I'm the &lt;g&gt;Giám đóc kinh doanh&lt;/g&gt; from ABC Company.
+Sales director
+Sales representative
+Sales Associate
+ </v>
+      </c>
+      <c r="I4" s="5" t="str">
         <v>**Prompt:**  
 You are an expert at creating English exercise content. You will receive `CẤU TRÚC`, `MAIN PHRASE`, and `OTHER PHRASE` inputs from the user.
 **Instructions:**  
@@ -583,10 +706,33 @@
 ]
 </v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="5" t="str" xml:space="preserve">
+        <v> { 
+ "structure": "I'm the ______ from ABC Company.", 
+"mainPhrase": "Sales representative", 
+ "optionalPhrase": "Sales director" 
+}</v>
+      </c>
+      <c r="K4" s="5" t="str">
+        <v>[
+ {
+ "sentence": "I'm the &lt;g&gt;Đại diện kinh doanh&lt;/g&gt; from ABC Company.",
+ "answer_1": "Sales representative", // main phrase
+ "answer_2": "Business representative",
+ "answer_3": "Sales agent",
+ "answer_2_description": "&lt;r&gt;Business representative&lt;/r&gt; không hoàn toàn đúng vì 'Business representative' thường mang nghĩa rộng hơn 'Đại diện kinh doanh', không chuyên biệt cho mảng bán hàng.",
+ "answer_3_description": "&lt;r&gt;Sales agent&lt;/r&gt; không hoàn toàn chính xác vì 'Sales agent' thường được dùng cho vai trò đại diện bán hàng theo hợp đồng, không bao hàm toàn bộ công việc của một 'Sales representative'."
+ },
+ {
+ "sentence": "I'm the &lt;g&gt;Giám đốc kinh doanh&lt;/g&gt; from ABC Company.",
+ "answer_1": "Sales director", // other phrase
+ "answer_2": "Sales manager",
+ "answer_3": "Commercial director",
+ "answer_2_description": "&lt;r&gt;Sales manager&lt;/r&gt; không hoàn toàn đúng vì 'Sales manager' mang nghĩa là 'Quản lý kinh doanh' thay vì 'Giám đốc kinh doanh', thể hiện cấp bậc thấp hơn trong cấu trúc công ty.",
+ "answer_3_description": "&lt;r&gt;Commercial director&lt;/r&gt; không chính xác vì 'Commercial director' quản lý các hoạt động thương mại nói chung, không chuyên biệt về kinh doanh hoặc bán hàng."
+ }
+]</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -595,19 +741,97 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="5">
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="G5" s="5" t="str" xml:space="preserve">
+        <v>Main phrase
+Optional phrase
+Sales representative
+Sales director
+Sales associate
+ </v>
+      </c>
+      <c r="H5" s="5" t="str" xml:space="preserve">
+        <v>description
+sentence_en
+sentence_vi
+ipa
+Hãy nói cụm sau
+Sales representative
+Đại diện kinh doanh
+/seɪlz ˌrɛprɪˈzɛn(t)ətɪv/
+Hãy nói cụm sau
+Sales director
+Giám đốc kinh doanh
+/seɪlz daɪˈrɛktər/
+Hãy nói cụm sau
+Sales Associate
+Nhân viên bán hàng
+/seɪlz əˈsoʊʃiət/
+ </v>
+      </c>
+      <c r="I5" s="5" t="str">
+        <v>**Prompt:**
+You are an expert at creating English exercise content. Given a "main phrase" and up to two optional phrases, generate a JSON array of objects where each object includes:
+- `sentence_en`: the English phrase
+- `sentence_vi`: the Vietnamese translation
+- `ipa`: the IPA pronunciation
+Response JSON format (not include other characters, such as ```JSON)
+**Example Input:**
+{
+    "main phrase": "Sales representative",
+    "optional phrase 1": "Sales director",
+    "optional phrase 2": "Sales associate"
+}
+**Expected Output:**
+[
+    {
+        "sentence_en": "Sales representative",
+        "sentence_vi": "Đại diện kinh doanh",
+        "ipa": "/seɪlz ˌrɛprɪˈzɛn(t)ətɪv/"
+    },
+    {
+        "sentence_en": "Sales director",
+        "sentence_vi": "Giám đốc kinh doanh",
+        "ipa": "/seɪlz daɪˈrɛktər/"
+    },
+    {
+        "sentence_en": "Sales Associate",
+        "sentence_vi": "Nhân viên bán hàng",
+        "ipa": "/seɪlz əˈsoʊʃiət/"
+    }
+]</v>
+      </c>
+      <c r="J5" s="5" t="str">
+        <v>promising start-upleading firmpioneer company</v>
+      </c>
+      <c r="K5" s="5" t="str">
+        <v>[
+  {
+    "sentence_en": "Promising start-up",
+    "sentence_vi": "Công ty khởi nghiệp đầy hứa hẹn",
+    "ipa": "/ˈprɒmɪsɪŋ ˈstɑːrt ʌp/"
+  },
+  {
+    "sentence_en": "Leading firm",
+    "sentence_vi": "Công ty hàng đầu",
+    "ipa": "/ˈliːdɪŋ fɜːrm/"
+  },
+  {
+    "sentence_en": "Pioneer company",
+    "sentence_vi": "Công ty tiên phong",
+    "ipa": "/ˌpaɪəˈnɪr ˈkʌmpəni/"
+  }
+]</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -616,19 +840,153 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="6">
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="G6" s="5" t="str" xml:space="preserve">
+        <v>Câu hỏi
+Cấu trúc
+Cụm thông tin
+Main phrase
+Optional phrase
+Which company are you working for?
+I'm the ______ from ABC Company. 
+Sales representative
+Sales director
+Sales associate
+ </v>
+      </c>
+      <c r="H6" s="5" t="str" xml:space="preserve">
+        <v>sentence_hide
+sentence_en
+sentence_vi
+I'm the Sales representative from ABC company.
+I'm the Sales representative from ABC company.
+Tôi là đại diện kinh doanh của công ty ABC.
+I'm the _____ ______________ from ABC company.
+I'm the Sales representative from ABC company.
+Tôi là đại diện kinh doanh của công ty ABC.
+I'm the _____ ________ from ABC company.
+I'm the Sales director from ABC company.
+Tôi là giám đốc kinh doanh của công ty ABC.
+I'm the _____ _________ from ABC company.
+I'm the Sales associate from ABC company.
+Tôi là nhân viên bán hàng của công ty ABC.
+___ ___ Sales representative from ABC company.
+I'm the Sales representative from ABC company.
+Tôi là đại diện kinh doanh của công ty ABC.
+___ ___ Sales director from ABC company.
+I'm the Sales director from ABC company.
+Tôi là giám đốc kinh doanh của công ty ABC.
+___ ___ Sales associate from ABC company.
+I'm the Sales associate from ABC company.
+Tôi là nhân viên bán hàng của công ty ABC.
+_____ _______ ___ ___ _______ ____?
+Which company are you working for?
+Bạn đang làm việc cho công ty nào vậy?
+ </v>
+      </c>
+      <c r="I6" s="5" t="str">
+        <v>**Prompt:**
+You are an expert at creating English exercise content. Based on the given structure, generate a JSON response with various English sentences, where specific words are hidden to create fill-in-the-blank exercises. Translate each sentence into Vietnamese.
+**Instruction:**
+- The output should contain 7 JSON objects within a JSON array.
+- JSON 1: Full sentence with no blanks.
+- JSONs 2, 3, 4: Replace each phrase in turn with underscores (one JSON per phrase).
+- JSONs 5, 6, 7: Only the specified phrases are visible, while the rest of the sentence is replaced by underscores.
+Response JSON format (not include other characters such as ```JSON)
+**Example Input:**
+Câu hỏi: Which company are you working for?  
+Cấu trúc: I'm the ______ from ABC Company.  
+Cụm thông tin: phrase 1, 2, 3: Sales representative, Sales director, Sales associate  
+**Expected Output:**
+[
+    {
+      "sentence_hide": "I'm the Sales representative from ABC company.",
+      "sentence_en": "I'm the Sales representative from ABC company.",
+      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+    },
+    {
+      "sentence_hide": "I'm the ____    _____ from ABC Company.", 
+      "sentence_en": "I'm the Sales representative from ABC company.",
+      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+    },
+    {
+      "sentence_hide": "I'm the _____ _____ from ABC company.", 
+      "sentence_en": "I'm the Sales director from ABC company.",
+      "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
+    },
+    {
+      "sentence_hide": "I'm the ___________ from ABC company.",
+      "sentence_en": "I'm the Sales associate from ABC company.",
+      "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
+    },
+    {
+      "sentence_hide": "___ ____ Sales representative from ABC company.", 
+      "sentence_en": "I'm the Sales representative from ABC company.",
+      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+    },
+    {
+      "sentence_hide": "___ ____ Sales director from ABC company.",
+      "sentence_en": "I'm the Sales director from ABC company.",
+      "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
+    },
+    {
+      "sentence_hide": "___ ____ Sales associate from ABC company.",
+      "sentence_en": "I'm the Sales associate from ABC company.",
+      "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
+    }
+]</v>
+      </c>
+      <c r="J6" s="5" t="str">
+        <v>What kind of business are you?We're a _____promising start-upleading firmpioneer company</v>
+      </c>
+      <c r="K6" s="5" t="str">
+        <v>[
+  {
+    "sentence_hide": "We're a promising start-up leading firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "We're a _____ start-up leading firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "We're a promising _____ leading firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "We're a promising start-up _____ firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "___ a promising start-up leading firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "___ a promising start-up _____ firm pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  },
+  {
+    "sentence_hide": "___ a promising start-up leading _____ pioneer company.",
+    "sentence_en": "We're a promising start-up leading firm pioneer company.",
+    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+  }
+]</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
@@ -637,19 +995,21 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="7">
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -658,19 +1018,21 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="8">
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -679,19 +1041,21 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="9">
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -700,19 +1064,21 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="10">
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -721,8 +1087,10 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="11">
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -742,8 +1110,10 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="12">
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -763,8 +1133,10 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="13">
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -784,8 +1156,10 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="14">
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -805,8 +1179,10 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="15">
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -826,8 +1202,10 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="16">
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -847,8 +1225,10 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="17">
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="17">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -868,8 +1248,10 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="18">
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -889,8 +1271,10 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="19">
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -910,8 +1294,10 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="20">
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -931,8 +1317,10 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="21">
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -952,8 +1340,10 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="22">
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -973,8 +1363,10 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="23">
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -994,8 +1386,10 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="24">
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1015,8 +1409,10 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="25">
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1036,8 +1432,10 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="26">
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1057,8 +1455,10 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="27">
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="27">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1078,8 +1478,10 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="28">
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1099,8 +1501,10 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="29">
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1120,8 +1524,10 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="30">
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="30">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1141,8 +1547,10 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="31">
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="31">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1162,8 +1570,10 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="32">
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="32">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1183,8 +1593,10 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="33">
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1204,8 +1616,10 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="34">
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1225,8 +1639,10 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="35">
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1246,8 +1662,10 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="36">
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1267,8 +1685,10 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="37">
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="37">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1288,8 +1708,10 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="38">
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="38">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1309,8 +1731,10 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="39">
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="39">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1330,8 +1754,10 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="40">
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="40">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1351,8 +1777,10 @@
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="41">
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1372,8 +1800,10 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="42">
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="42">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1393,8 +1823,10 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="43">
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="43">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1414,8 +1846,10 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="44">
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="44">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1435,8 +1869,10 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="45">
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="45">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1456,8 +1892,10 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="46">
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="46">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1477,8 +1915,10 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="47">
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="47">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1498,8 +1938,10 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="48">
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="48">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1519,8 +1961,10 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="49">
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="49">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1540,8 +1984,10 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="50">
+      <c r="T49" s="1"/>
+      <c r="U49" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="50">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1561,8 +2007,10 @@
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="51">
+      <c r="T50" s="1"/>
+      <c r="U50" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="51">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1582,8 +2030,10 @@
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="52">
+      <c r="T51" s="1"/>
+      <c r="U51" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="52">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1603,8 +2053,10 @@
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="53">
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="53">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1624,8 +2076,10 @@
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="54">
+      <c r="T53" s="1"/>
+      <c r="U53" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="54">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1645,8 +2099,10 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="55">
+      <c r="T54" s="1"/>
+      <c r="U54" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="55">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1666,8 +2122,10 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="56">
+      <c r="T55" s="1"/>
+      <c r="U55" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="56">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1687,8 +2145,10 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="57">
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="57">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1708,8 +2168,10 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="58">
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="58">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1729,8 +2191,10 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="59">
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="59">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1750,8 +2214,10 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="60">
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="60">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1771,8 +2237,10 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="61">
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="61">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1792,8 +2260,10 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="62">
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="62">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1813,8 +2283,10 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="63">
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="63">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1834,8 +2306,10 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="64">
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="64">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1855,8 +2329,10 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="65">
+      <c r="T64" s="1"/>
+      <c r="U64" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="65">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1876,8 +2352,10 @@
       <c r="Q65" s="1"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="66">
+      <c r="T65" s="1"/>
+      <c r="U65" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="66">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1897,8 +2375,10 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="67">
+      <c r="T66" s="1"/>
+      <c r="U66" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="67">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1918,8 +2398,10 @@
       <c r="Q67" s="1"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="68">
+      <c r="T67" s="1"/>
+      <c r="U67" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="68">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1939,8 +2421,10 @@
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="69">
+      <c r="T68" s="1"/>
+      <c r="U68" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="69">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1960,8 +2444,10 @@
       <c r="Q69" s="1"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="70">
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="70">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1981,8 +2467,10 @@
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="71">
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="71">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2002,8 +2490,10 @@
       <c r="Q71" s="1"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="72">
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="72">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2023,8 +2513,10 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="73">
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="73">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2044,8 +2536,10 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="74">
+      <c r="T73" s="1"/>
+      <c r="U73" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="74">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2065,8 +2559,10 @@
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="75">
+      <c r="T74" s="1"/>
+      <c r="U74" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="75">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2086,8 +2582,10 @@
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="76">
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="76">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2107,8 +2605,10 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="77">
+      <c r="T76" s="1"/>
+      <c r="U76" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="77">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2128,8 +2628,10 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="78">
+      <c r="T77" s="1"/>
+      <c r="U77" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="78">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2149,8 +2651,10 @@
       <c r="Q78" s="1"/>
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="79">
+      <c r="T78" s="1"/>
+      <c r="U78" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="79">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2170,8 +2674,10 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="80">
+      <c r="T79" s="1"/>
+      <c r="U79" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="80">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2191,8 +2697,10 @@
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="81">
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="81">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2212,8 +2720,10 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="82">
+      <c r="T81" s="1"/>
+      <c r="U81" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="82">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2233,8 +2743,10 @@
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="83">
+      <c r="T82" s="1"/>
+      <c r="U82" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="83">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2254,8 +2766,10 @@
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="84">
+      <c r="T83" s="1"/>
+      <c r="U83" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="84">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2275,8 +2789,10 @@
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="85">
+      <c r="T84" s="1"/>
+      <c r="U84" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="85">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2296,8 +2812,10 @@
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="86">
+      <c r="T85" s="1"/>
+      <c r="U85" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="86">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2317,8 +2835,10 @@
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="87">
+      <c r="T86" s="1"/>
+      <c r="U86" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="87">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2338,8 +2858,10 @@
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="88">
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="88">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2359,8 +2881,10 @@
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="89">
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="89">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2380,8 +2904,10 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="90">
+      <c r="T89" s="1"/>
+      <c r="U89" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="90">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2401,8 +2927,10 @@
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="91">
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="91">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2422,8 +2950,10 @@
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="92">
+      <c r="T91" s="1"/>
+      <c r="U91" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="92">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2443,8 +2973,10 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="93">
+      <c r="T92" s="1"/>
+      <c r="U92" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="93">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2464,8 +2996,10 @@
       <c r="Q93" s="1"/>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="94">
+      <c r="T93" s="1"/>
+      <c r="U93" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="94">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2485,8 +3019,10 @@
       <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="95">
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="95">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2506,8 +3042,10 @@
       <c r="Q95" s="1"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="96">
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="96">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2527,8 +3065,10 @@
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="97">
+      <c r="T96" s="1"/>
+      <c r="U96" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="97">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2548,8 +3088,10 @@
       <c r="Q97" s="1"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="98">
+      <c r="T97" s="1"/>
+      <c r="U97" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="98">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2569,8 +3111,10 @@
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="99">
+      <c r="T98" s="1"/>
+      <c r="U98" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="99">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2590,8 +3134,10 @@
       <c r="Q99" s="1"/>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="100">
+      <c r="T99" s="1"/>
+      <c r="U99" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="100">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2611,8 +3157,10 @@
       <c r="Q100" s="1"/>
       <c r="R100" s="1"/>
       <c r="S100" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="101">
+      <c r="T100" s="1"/>
+      <c r="U100" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="101">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2632,8 +3180,10 @@
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="102">
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="102">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2653,8 +3203,10 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="103">
+      <c r="T102" s="1"/>
+      <c r="U102" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="103">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2674,8 +3226,10 @@
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="104">
+      <c r="T103" s="1"/>
+      <c r="U103" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="104">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2695,8 +3249,10 @@
       <c r="Q104" s="1"/>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="105">
+      <c r="T104" s="1"/>
+      <c r="U104" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="105">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2716,8 +3272,10 @@
       <c r="Q105" s="1"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="106">
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="106">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2737,8 +3295,10 @@
       <c r="Q106" s="1"/>
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="107">
+      <c r="T106" s="1"/>
+      <c r="U106" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="107">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2758,8 +3318,10 @@
       <c r="Q107" s="1"/>
       <c r="R107" s="1"/>
       <c r="S107" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="108">
+      <c r="T107" s="1"/>
+      <c r="U107" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="108">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2779,8 +3341,10 @@
       <c r="Q108" s="1"/>
       <c r="R108" s="1"/>
       <c r="S108" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="109">
+      <c r="T108" s="1"/>
+      <c r="U108" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="109">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2800,8 +3364,10 @@
       <c r="Q109" s="1"/>
       <c r="R109" s="1"/>
       <c r="S109" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="110">
+      <c r="T109" s="1"/>
+      <c r="U109" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="110">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2821,8 +3387,10 @@
       <c r="Q110" s="1"/>
       <c r="R110" s="1"/>
       <c r="S110" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="111">
+      <c r="T110" s="1"/>
+      <c r="U110" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="111">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2842,8 +3410,10 @@
       <c r="Q111" s="1"/>
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="112">
+      <c r="T111" s="1"/>
+      <c r="U111" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="112">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2863,8 +3433,10 @@
       <c r="Q112" s="1"/>
       <c r="R112" s="1"/>
       <c r="S112" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="113">
+      <c r="T112" s="1"/>
+      <c r="U112" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="113">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2884,8 +3456,10 @@
       <c r="Q113" s="1"/>
       <c r="R113" s="1"/>
       <c r="S113" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="114">
+      <c r="T113" s="1"/>
+      <c r="U113" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="114">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2905,8 +3479,10 @@
       <c r="Q114" s="1"/>
       <c r="R114" s="1"/>
       <c r="S114" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="115">
+      <c r="T114" s="1"/>
+      <c r="U114" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="115">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2926,8 +3502,10 @@
       <c r="Q115" s="1"/>
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="116">
+      <c r="T115" s="1"/>
+      <c r="U115" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="116">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2947,8 +3525,10 @@
       <c r="Q116" s="1"/>
       <c r="R116" s="1"/>
       <c r="S116" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="117">
+      <c r="T116" s="1"/>
+      <c r="U116" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="117">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2968,8 +3548,10 @@
       <c r="Q117" s="1"/>
       <c r="R117" s="1"/>
       <c r="S117" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="118">
+      <c r="T117" s="1"/>
+      <c r="U117" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="118">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2989,8 +3571,10 @@
       <c r="Q118" s="1"/>
       <c r="R118" s="1"/>
       <c r="S118" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="119">
+      <c r="T118" s="1"/>
+      <c r="U118" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="119">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3010,8 +3594,10 @@
       <c r="Q119" s="1"/>
       <c r="R119" s="1"/>
       <c r="S119" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="120">
+      <c r="T119" s="1"/>
+      <c r="U119" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="120">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3031,8 +3617,10 @@
       <c r="Q120" s="1"/>
       <c r="R120" s="1"/>
       <c r="S120" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="121">
+      <c r="T120" s="1"/>
+      <c r="U120" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="121">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3052,8 +3640,10 @@
       <c r="Q121" s="1"/>
       <c r="R121" s="1"/>
       <c r="S121" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="122">
+      <c r="T121" s="1"/>
+      <c r="U121" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="122">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3073,8 +3663,10 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="123">
+      <c r="T122" s="1"/>
+      <c r="U122" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="123">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3094,8 +3686,10 @@
       <c r="Q123" s="1"/>
       <c r="R123" s="1"/>
       <c r="S123" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="124">
+      <c r="T123" s="1"/>
+      <c r="U123" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="124">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3115,8 +3709,10 @@
       <c r="Q124" s="1"/>
       <c r="R124" s="1"/>
       <c r="S124" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="125">
+      <c r="T124" s="1"/>
+      <c r="U124" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="125">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3136,8 +3732,10 @@
       <c r="Q125" s="1"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="126">
+      <c r="T125" s="1"/>
+      <c r="U125" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="126">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3157,8 +3755,10 @@
       <c r="Q126" s="1"/>
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="127">
+      <c r="T126" s="1"/>
+      <c r="U126" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="127">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3178,8 +3778,10 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
       <c r="S127" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="128">
+      <c r="T127" s="1"/>
+      <c r="U127" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="128">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3199,8 +3801,10 @@
       <c r="Q128" s="1"/>
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="129">
+      <c r="T128" s="1"/>
+      <c r="U128" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="129">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3220,8 +3824,10 @@
       <c r="Q129" s="1"/>
       <c r="R129" s="1"/>
       <c r="S129" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="130">
+      <c r="T129" s="1"/>
+      <c r="U129" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="130">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3241,8 +3847,10 @@
       <c r="Q130" s="1"/>
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="131">
+      <c r="T130" s="1"/>
+      <c r="U130" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="131">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3262,8 +3870,10 @@
       <c r="Q131" s="1"/>
       <c r="R131" s="1"/>
       <c r="S131" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="132">
+      <c r="T131" s="1"/>
+      <c r="U131" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="132">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3283,8 +3893,10 @@
       <c r="Q132" s="1"/>
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="133">
+      <c r="T132" s="1"/>
+      <c r="U132" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="133">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3304,8 +3916,10 @@
       <c r="Q133" s="1"/>
       <c r="R133" s="1"/>
       <c r="S133" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="134">
+      <c r="T133" s="1"/>
+      <c r="U133" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="134">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3325,8 +3939,10 @@
       <c r="Q134" s="1"/>
       <c r="R134" s="1"/>
       <c r="S134" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="135">
+      <c r="T134" s="1"/>
+      <c r="U134" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="135">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3346,8 +3962,10 @@
       <c r="Q135" s="1"/>
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="136">
+      <c r="T135" s="1"/>
+      <c r="U135" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="136">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3367,8 +3985,10 @@
       <c r="Q136" s="1"/>
       <c r="R136" s="1"/>
       <c r="S136" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="137">
+      <c r="T136" s="1"/>
+      <c r="U136" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="137">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3388,8 +4008,10 @@
       <c r="Q137" s="1"/>
       <c r="R137" s="1"/>
       <c r="S137" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="138">
+      <c r="T137" s="1"/>
+      <c r="U137" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="138">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3409,8 +4031,10 @@
       <c r="Q138" s="1"/>
       <c r="R138" s="1"/>
       <c r="S138" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="139">
+      <c r="T138" s="1"/>
+      <c r="U138" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="139">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3430,8 +4054,10 @@
       <c r="Q139" s="1"/>
       <c r="R139" s="1"/>
       <c r="S139" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="140">
+      <c r="T139" s="1"/>
+      <c r="U139" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="140">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3451,8 +4077,10 @@
       <c r="Q140" s="1"/>
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="141">
+      <c r="T140" s="1"/>
+      <c r="U140" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="141">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3472,8 +4100,10 @@
       <c r="Q141" s="1"/>
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="142">
+      <c r="T141" s="1"/>
+      <c r="U141" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="142">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3493,8 +4123,10 @@
       <c r="Q142" s="1"/>
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="143">
+      <c r="T142" s="1"/>
+      <c r="U142" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="143">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3514,8 +4146,10 @@
       <c r="Q143" s="1"/>
       <c r="R143" s="1"/>
       <c r="S143" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="144">
+      <c r="T143" s="1"/>
+      <c r="U143" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="144">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3535,8 +4169,10 @@
       <c r="Q144" s="1"/>
       <c r="R144" s="1"/>
       <c r="S144" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="145">
+      <c r="T144" s="1"/>
+      <c r="U144" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="145">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3556,8 +4192,10 @@
       <c r="Q145" s="1"/>
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="146">
+      <c r="T145" s="1"/>
+      <c r="U145" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="146">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3577,8 +4215,10 @@
       <c r="Q146" s="1"/>
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="147">
+      <c r="T146" s="1"/>
+      <c r="U146" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="147">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3598,8 +4238,10 @@
       <c r="Q147" s="1"/>
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="148">
+      <c r="T147" s="1"/>
+      <c r="U147" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="148">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3619,8 +4261,10 @@
       <c r="Q148" s="1"/>
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="149">
+      <c r="T148" s="1"/>
+      <c r="U148" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="149">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3640,8 +4284,10 @@
       <c r="Q149" s="1"/>
       <c r="R149" s="1"/>
       <c r="S149" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="150">
+      <c r="T149" s="1"/>
+      <c r="U149" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="150">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3661,8 +4307,10 @@
       <c r="Q150" s="1"/>
       <c r="R150" s="1"/>
       <c r="S150" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="151">
+      <c r="T150" s="1"/>
+      <c r="U150" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="151">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3682,8 +4330,10 @@
       <c r="Q151" s="1"/>
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="152">
+      <c r="T151" s="1"/>
+      <c r="U151" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="152">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3703,8 +4353,10 @@
       <c r="Q152" s="1"/>
       <c r="R152" s="1"/>
       <c r="S152" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="153">
+      <c r="T152" s="1"/>
+      <c r="U152" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="153">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3724,8 +4376,10 @@
       <c r="Q153" s="1"/>
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="154">
+      <c r="T153" s="1"/>
+      <c r="U153" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="154">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3745,8 +4399,10 @@
       <c r="Q154" s="1"/>
       <c r="R154" s="1"/>
       <c r="S154" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="155">
+      <c r="T154" s="1"/>
+      <c r="U154" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="155">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3766,8 +4422,10 @@
       <c r="Q155" s="1"/>
       <c r="R155" s="1"/>
       <c r="S155" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="156">
+      <c r="T155" s="1"/>
+      <c r="U155" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="156">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3787,8 +4445,10 @@
       <c r="Q156" s="1"/>
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="157">
+      <c r="T156" s="1"/>
+      <c r="U156" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="157">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3808,8 +4468,10 @@
       <c r="Q157" s="1"/>
       <c r="R157" s="1"/>
       <c r="S157" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="158">
+      <c r="T157" s="1"/>
+      <c r="U157" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="158">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3829,8 +4491,10 @@
       <c r="Q158" s="1"/>
       <c r="R158" s="1"/>
       <c r="S158" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="159">
+      <c r="T158" s="1"/>
+      <c r="U158" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="159">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3850,8 +4514,10 @@
       <c r="Q159" s="1"/>
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="160">
+      <c r="T159" s="1"/>
+      <c r="U159" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="160">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3871,8 +4537,10 @@
       <c r="Q160" s="1"/>
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="161">
+      <c r="T160" s="1"/>
+      <c r="U160" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="161">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3892,8 +4560,10 @@
       <c r="Q161" s="1"/>
       <c r="R161" s="1"/>
       <c r="S161" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="162">
+      <c r="T161" s="1"/>
+      <c r="U161" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="162">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3913,8 +4583,10 @@
       <c r="Q162" s="1"/>
       <c r="R162" s="1"/>
       <c r="S162" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="163">
+      <c r="T162" s="1"/>
+      <c r="U162" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="163">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3934,8 +4606,10 @@
       <c r="Q163" s="1"/>
       <c r="R163" s="1"/>
       <c r="S163" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="164">
+      <c r="T163" s="1"/>
+      <c r="U163" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="164">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3955,8 +4629,10 @@
       <c r="Q164" s="1"/>
       <c r="R164" s="1"/>
       <c r="S164" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="165">
+      <c r="T164" s="1"/>
+      <c r="U164" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="165">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3976,8 +4652,10 @@
       <c r="Q165" s="1"/>
       <c r="R165" s="1"/>
       <c r="S165" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="166">
+      <c r="T165" s="1"/>
+      <c r="U165" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="166">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3997,8 +4675,10 @@
       <c r="Q166" s="1"/>
       <c r="R166" s="1"/>
       <c r="S166" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="167">
+      <c r="T166" s="1"/>
+      <c r="U166" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="167">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4018,8 +4698,10 @@
       <c r="Q167" s="1"/>
       <c r="R167" s="1"/>
       <c r="S167" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="168">
+      <c r="T167" s="1"/>
+      <c r="U167" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="168">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4039,8 +4721,10 @@
       <c r="Q168" s="1"/>
       <c r="R168" s="1"/>
       <c r="S168" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="169">
+      <c r="T168" s="1"/>
+      <c r="U168" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="169">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4060,8 +4744,10 @@
       <c r="Q169" s="1"/>
       <c r="R169" s="1"/>
       <c r="S169" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="170">
+      <c r="T169" s="1"/>
+      <c r="U169" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="170">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4081,8 +4767,10 @@
       <c r="Q170" s="1"/>
       <c r="R170" s="1"/>
       <c r="S170" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="171">
+      <c r="T170" s="1"/>
+      <c r="U170" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="171">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4102,8 +4790,10 @@
       <c r="Q171" s="1"/>
       <c r="R171" s="1"/>
       <c r="S171" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="172">
+      <c r="T171" s="1"/>
+      <c r="U171" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="172">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4123,8 +4813,10 @@
       <c r="Q172" s="1"/>
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="173">
+      <c r="T172" s="1"/>
+      <c r="U172" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="173">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4144,8 +4836,10 @@
       <c r="Q173" s="1"/>
       <c r="R173" s="1"/>
       <c r="S173" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="174">
+      <c r="T173" s="1"/>
+      <c r="U173" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="174">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4165,8 +4859,10 @@
       <c r="Q174" s="1"/>
       <c r="R174" s="1"/>
       <c r="S174" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="175">
+      <c r="T174" s="1"/>
+      <c r="U174" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="175">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4186,8 +4882,10 @@
       <c r="Q175" s="1"/>
       <c r="R175" s="1"/>
       <c r="S175" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="176">
+      <c r="T175" s="1"/>
+      <c r="U175" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="176">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4207,8 +4905,10 @@
       <c r="Q176" s="1"/>
       <c r="R176" s="1"/>
       <c r="S176" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="177">
+      <c r="T176" s="1"/>
+      <c r="U176" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="177">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4228,8 +4928,10 @@
       <c r="Q177" s="1"/>
       <c r="R177" s="1"/>
       <c r="S177" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="178">
+      <c r="T177" s="1"/>
+      <c r="U177" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="178">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4249,8 +4951,10 @@
       <c r="Q178" s="1"/>
       <c r="R178" s="1"/>
       <c r="S178" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="179">
+      <c r="T178" s="1"/>
+      <c r="U178" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="179">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4270,8 +4974,10 @@
       <c r="Q179" s="1"/>
       <c r="R179" s="1"/>
       <c r="S179" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="180">
+      <c r="T179" s="1"/>
+      <c r="U179" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="180">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4291,8 +4997,10 @@
       <c r="Q180" s="1"/>
       <c r="R180" s="1"/>
       <c r="S180" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="181">
+      <c r="T180" s="1"/>
+      <c r="U180" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="181">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4312,8 +5020,10 @@
       <c r="Q181" s="1"/>
       <c r="R181" s="1"/>
       <c r="S181" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="182">
+      <c r="T181" s="1"/>
+      <c r="U181" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="182">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4333,8 +5043,10 @@
       <c r="Q182" s="1"/>
       <c r="R182" s="1"/>
       <c r="S182" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="183">
+      <c r="T182" s="1"/>
+      <c r="U182" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="183">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4354,8 +5066,10 @@
       <c r="Q183" s="1"/>
       <c r="R183" s="1"/>
       <c r="S183" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="184">
+      <c r="T183" s="1"/>
+      <c r="U183" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="184">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -4375,8 +5089,10 @@
       <c r="Q184" s="1"/>
       <c r="R184" s="1"/>
       <c r="S184" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="185">
+      <c r="T184" s="1"/>
+      <c r="U184" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="185">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -4396,8 +5112,10 @@
       <c r="Q185" s="1"/>
       <c r="R185" s="1"/>
       <c r="S185" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="186">
+      <c r="T185" s="1"/>
+      <c r="U185" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="186">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -4417,8 +5135,10 @@
       <c r="Q186" s="1"/>
       <c r="R186" s="1"/>
       <c r="S186" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="187">
+      <c r="T186" s="1"/>
+      <c r="U186" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="187">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -4438,8 +5158,10 @@
       <c r="Q187" s="1"/>
       <c r="R187" s="1"/>
       <c r="S187" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="188">
+      <c r="T187" s="1"/>
+      <c r="U187" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="188">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -4459,8 +5181,10 @@
       <c r="Q188" s="1"/>
       <c r="R188" s="1"/>
       <c r="S188" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="189">
+      <c r="T188" s="1"/>
+      <c r="U188" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="189">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -4480,8 +5204,10 @@
       <c r="Q189" s="1"/>
       <c r="R189" s="1"/>
       <c r="S189" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="190">
+      <c r="T189" s="1"/>
+      <c r="U189" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="190">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -4501,8 +5227,10 @@
       <c r="Q190" s="1"/>
       <c r="R190" s="1"/>
       <c r="S190" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="191">
+      <c r="T190" s="1"/>
+      <c r="U190" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="191">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -4522,8 +5250,10 @@
       <c r="Q191" s="1"/>
       <c r="R191" s="1"/>
       <c r="S191" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="192">
+      <c r="T191" s="1"/>
+      <c r="U191" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="192">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -4543,8 +5273,10 @@
       <c r="Q192" s="1"/>
       <c r="R192" s="1"/>
       <c r="S192" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="193">
+      <c r="T192" s="1"/>
+      <c r="U192" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="193">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -4564,8 +5296,10 @@
       <c r="Q193" s="1"/>
       <c r="R193" s="1"/>
       <c r="S193" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="194">
+      <c r="T193" s="1"/>
+      <c r="U193" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="194">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -4585,8 +5319,10 @@
       <c r="Q194" s="1"/>
       <c r="R194" s="1"/>
       <c r="S194" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="195">
+      <c r="T194" s="1"/>
+      <c r="U194" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="195">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -4606,8 +5342,10 @@
       <c r="Q195" s="1"/>
       <c r="R195" s="1"/>
       <c r="S195" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="196">
+      <c r="T195" s="1"/>
+      <c r="U195" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="196">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -4627,8 +5365,10 @@
       <c r="Q196" s="1"/>
       <c r="R196" s="1"/>
       <c r="S196" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="197">
+      <c r="T196" s="1"/>
+      <c r="U196" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="197">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -4648,8 +5388,10 @@
       <c r="Q197" s="1"/>
       <c r="R197" s="1"/>
       <c r="S197" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="198">
+      <c r="T197" s="1"/>
+      <c r="U197" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="198">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -4669,8 +5411,10 @@
       <c r="Q198" s="1"/>
       <c r="R198" s="1"/>
       <c r="S198" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="199">
+      <c r="T198" s="1"/>
+      <c r="U198" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="199">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -4690,8 +5434,10 @@
       <c r="Q199" s="1"/>
       <c r="R199" s="1"/>
       <c r="S199" s="1"/>
-    </row>
-    <row customHeight="true" ht="41" r="200">
+      <c r="T199" s="1"/>
+      <c r="U199" s="1"/>
+    </row>
+    <row customHeight="true" ht="113" r="200">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -4711,6 +5457,8 @@
       <c r="Q200" s="1"/>
       <c r="R200" s="1"/>
       <c r="S200" s="1"/>
+      <c r="T200" s="1"/>
+      <c r="U200" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Fix bug: 2 nút Copy - Done 2 dạng đầu - sẵn sàng cho deploy1
</commit_message>
<xml_diff>
--- a/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
+++ b/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
@@ -102,13 +102,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF5EB"/>
+        <fgColor rgb="FFD5F6F2"/>
         <bgColor/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD5F6F2"/>
+        <fgColor rgb="FFFFF5EB"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -173,10 +173,10 @@
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -528,47 +528,47 @@
   </cols>
   <sheetData>
     <row customHeight="true" ht="40" r="1">
-      <c r="A1" s="3" t="str">
+      <c r="A1" s="5" t="str">
         <v>Công việc</v>
       </c>
-      <c r="B1" s="3" t="str">
+      <c r="B1" s="5" t="str">
         <v>Input</v>
       </c>
-      <c r="C1" s="3" t="str">
+      <c r="C1" s="5" t="str">
         <v>Output</v>
       </c>
-      <c r="D1" s="3" t="str">
+      <c r="D1" s="5" t="str">
         <v>Tham khảo</v>
       </c>
-      <c r="E1" s="3" t="str">
+      <c r="E1" s="5" t="str">
         <v>Prompt của a Hoàng</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4" t="str">
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="str">
         <v>input raw - từ Excel</v>
       </c>
-      <c r="H1" s="4" t="str">
+      <c r="H1" s="3" t="str">
         <v>output raw - từ Excel</v>
       </c>
-      <c r="I1" s="4" t="str">
+      <c r="I1" s="3" t="str">
         <v>prompt Cường</v>
       </c>
-      <c r="J1" s="4" t="str">
+      <c r="J1" s="3" t="str">
         <v>user_input - THOẢI MÁI, KO CẦN THEO JSON</v>
       </c>
-      <c r="K1" s="4" t="str">
+      <c r="K1" s="3" t="str">
         <v>output</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
     </row>
     <row customHeight="true" ht="113" r="2">
       <c r="A2" s="1"/>
@@ -779,39 +779,48 @@
  </v>
       </c>
       <c r="I5" s="2" t="str">
-        <v>**Prompt:**
-You are an expert at creating English exercise content. Given a "main phrase" and up to two optional phrases, generate a JSON array of objects where each object includes:
-- `sentence_en`: the English phrase
-- `sentence_vi`: the Vietnamese translation
-- `ipa`: the IPA pronunciation
-Response JSON format (not include other characters, such as ```JSON)
+        <v>You are an English exercise content expert. Given structure_en, main_phrase, and up to two optional_phrases, create a JSON array with:
+- sentence_en: English sentence
+- sentence_vi: Vietnamese translation
+- ipa: IPA pronunciation
+**Response Format:** Output only in JSON format with no extra characters  (such as ```Json) .
 **Example Input:**
 {
-    "main phrase": "Sales representative",
-    "optional phrase 1": "Sales director",
-    "optional phrase 2": "Sales associate"
+    "structure_en": "Our team of _____ specialists is here to help",
+    "main_phrase": "healthcare",
+    "optional_phrase_1": "financial",
+    "optional_phrase_2": "legal"
 }
 **Expected Output:**
 [
     {
-        "sentence_en": "Sales representative",
-        "sentence_vi": "Đại diện kinh doanh",
-        "ipa": "/seɪlz ˌrɛprɪˈzɛn(t)ətɪv/"
+        "sentence_en": "Our team of _____ specialists is here to help",
+        "sentence_vi": "Đội ngũ chuyên gia _____ của chúng tôi sẵn sàng hỗ trợ",
+        "ipa": "/ˈaʊər tiːm əv _____ ˈspɛʃəlɪsts ɪz hɪər tuː hɛlp/"
     },
     {
-        "sentence_en": "Sales director",
-        "sentence_vi": "Giám đốc kinh doanh",
-        "ipa": "/seɪlz daɪˈrɛktər/"
+        "sentence_en": "healthcare specialists",
+        "sentence_vi": "chuyên gia y tế",
+        "ipa": "/ˈhɛlθˌkɛr ˈspɛʃəlɪsts/"
     },
     {
-        "sentence_en": "Sales Associate",
-        "sentence_vi": "Nhân viên bán hàng",
-        "ipa": "/seɪlz əˈsoʊʃiət/"
+        "sentence_en": "financial specialists",
+        "sentence_vi": "chuyên gia tài chính",
+        "ipa": "/faɪˈnænʃəl ˈspɛʃəlɪsts/"
+    },
+    {
+        "sentence_en": "legal specialists",
+        "sentence_vi": "chuyên gia pháp lý",
+        "ipa": "/ˈliːɡəl ˈspɛʃəlɪsts/"
     }
 ]</v>
       </c>
-      <c r="J5" s="2" t="str">
-        <v>promising start-upleading firmpioneer company</v>
+      <c r="J5" s="2" t="str" xml:space="preserve">
+        <v>We're a _____
+promising start-up
+leading firm
+pioneer company 
+ </v>
       </c>
       <c r="K5" s="2" t="str">
         <v>[

</xml_diff>

<commit_message>
10H REFACTOR CODE (chia scripts.js thành các dạng bài RIÊNG) - KO HIỂU SAO - LÚC CHẠY - LÚC KO CHẠY) - CHẠY RỒI - BUG FIX 5 H - FIX XONG VẪN KO BIẾT SAO FIX ĐƯỢC
</commit_message>
<xml_diff>
--- a/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
+++ b/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <pane state="frozen" topLeftCell="A2" ySplit="1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
@@ -903,96 +903,128 @@
  </v>
       </c>
       <c r="I6" s="2" t="str">
-        <v>**Prompt:**
+        <v>
+**Prompt:**
 You are an expert at creating English exercise content. Based on the given structure, generate a JSON response with various English sentences, where specific words are hidden to create fill-in-the-blank exercises. Translate each sentence into Vietnamese.
 **Instruction:**
-- The output should contain 7 JSON objects within a JSON array.
+- The output should contain 8 JSON objects within a JSON array.
 - JSON 1: Full sentence with no blanks.
 - JSONs 2, 3, 4: Replace each phrase in turn with underscores (one JSON per phrase).
 - JSONs 5, 6, 7: Only the specified phrases are visible, while the rest of the sentence is replaced by underscores.
-Response JSON format (not include other characters such as ```JSON)
+- JSON 8: Full sentence with all words replaced by blanks.
+**Important**: In each `sentence_hide` field, ensure the length of underscores (`_____`) matches the number of characters of the hidden word(s).
+**Response JSON format (no additional characters like ```JSON)**
 **Example Input:**
-Câu hỏi: Which company are you working for?  
-Cấu trúc: I'm the ______ from ABC Company.  
-Cụm thông tin: phrase 1, 2, 3: Sales representative, Sales director, Sales associate  
+- **Question**: "Which company are you working for?"
+- **Structure**: "I'm the ______ from ABC Company."
+- **Phrases**: "Sales representative", "Sales director", "Sales associate"
 **Expected Output:**
 [
     {
-      "sentence_hide": "I'm the Sales representative from ABC company.",
-      "sentence_en": "I'm the Sales representative from ABC company.",
-      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+        "description": "Hãy nghe mình nói và đọc lại",
+        "sentence_hide": "I'm the Sales representative from ABC company.",
+        "sentence_en": "I'm the Sales representative from ABC company.",
+        "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
     },
     {
-      "sentence_hide": "I'm the ____    _____ from ABC Company.", 
-      "sentence_en": "I'm the Sales representative from ABC company.",
-      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+        "description": "Nhắc lại nhé",
+        "sentence_hide": "I'm the _____ _____________ from ABC company.",
+        "sentence_en": "I'm the Sales representative from ABC company.",
+        "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
     },
     {
-      "sentence_hide": "I'm the _____ _____ from ABC company.", 
-      "sentence_en": "I'm the Sales director from ABC company.",
-      "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "I'm the _____ _________ from ABC company.",
+        "sentence_en": "I'm the Sales director from ABC company.",
+        "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
     },
     {
-      "sentence_hide": "I'm the ___________ from ABC company.",
-      "sentence_en": "I'm the Sales associate from ABC company.",
-      "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "I'm the _____ _________ from ABC company.",
+        "sentence_en": "I'm the Sales associate from ABC company.",
+        "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
     },
     {
-      "sentence_hide": "___ ____ Sales representative from ABC company.", 
-      "sentence_en": "I'm the Sales representative from ABC company.",
-      "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "___ ___ Sales representative from ABC company.",
+        "sentence_en": "I'm the Sales representative from ABC company.",
+        "sentence_vi": "Tôi là đại diện kinh doanh của công ty ABC."
     },
     {
-      "sentence_hide": "___ ____ Sales director from ABC company.",
-      "sentence_en": "I'm the Sales director from ABC company.",
-      "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "___ ___ Sales director from ABC company.",
+        "sentence_en": "I'm the Sales director from ABC company.",
+        "sentence_vi": "Tôi là giám đốc kinh doanh của công ty ABC."
     },
     {
-      "sentence_hide": "___ ____ Sales associate from ABC company.",
-      "sentence_en": "I'm the Sales associate from ABC company.",
-      "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "___ ___ Sales associate from ABC company.",
+        "sentence_en": "I'm the Sales associate from ABC company.",
+        "sentence_vi": "Tôi là nhân viên bán hàng của công ty ABC."
+    },
+    {
+        "description": "Hãy dịch câu sau",
+        "sentence_hide": "_____ _______ ___ ___ _______ ____?",
+        "sentence_en": "Which company are you working for?",
+        "sentence_vi": "Bạn đang làm việc cho công ty nào vậy?"
     }
 ]</v>
       </c>
       <c r="J6" s="2" t="str">
-        <v>What kind of business are you?We're a _____promising start-upleading firmpioneer company</v>
+        <v>I’ll follow up with you ________
+next week
+tomorrow 
+afternoonon Wednesday</v>
       </c>
       <c r="K6" s="2" t="str">
         <v>[
   {
-    "sentence_hide": "We're a promising start-up leading firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy nghe mình nói và đọc lại",
+    "sentence_hide": "I’ll follow up with you next week.",
+    "sentence_en": "I’ll follow up with you next week.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào tuần tới."
   },
   {
-    "sentence_hide": "We're a _____ start-up leading firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Nhắc lại nhé",
+    "sentence_hide": "I’ll follow up with you _____ ____.",
+    "sentence_en": "I’ll follow up with you next week.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào tuần tới."
   },
   {
-    "sentence_hide": "We're a promising _____ leading firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll follow up with you ________.",
+    "sentence_en": "I’ll follow up with you tomorrow.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào ngày mai."
   },
   {
-    "sentence_hide": "We're a promising start-up _____ firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll follow up with you ____________.",
+    "sentence_en": "I’ll follow up with you on Wednesday.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào thứ Tư."
   },
   {
-    "sentence_hide": "___ a promising start-up leading firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll follow up with you ___ ____.",
+    "sentence_en": "I’ll follow up with you next week.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào tuần tới."
   },
   {
-    "sentence_hide": "___ a promising start-up _____ firm pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll follow up with you ___ ______.",
+    "sentence_en": "I’ll follow up with you tomorrow.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào ngày mai."
   },
   {
-    "sentence_hide": "___ a promising start-up leading _____ pioneer company.",
-    "sentence_en": "We're a promising start-up leading firm pioneer company.",
-    "sentence_vi": "Chúng tôi là một công ty khởi nghiệp đầy hứa hẹn, công ty dẫn đầu."
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll follow up with you __ ____________.",
+    "sentence_en": "I’ll follow up with you on Wednesday.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào thứ Tư."
+  },
+  {
+    "description": "Hãy dịch câu sau",
+    "sentence_hide": "I’ll ______ __ ____ ____?",
+    "sentence_en": "I’ll follow up with you next week.",
+    "sentence_vi": "Tôi sẽ theo dõi bạn vào tuần tới."
   }
 ]</v>
       </c>
@@ -1014,10 +1046,68 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="G7" s="2" t="str">
+        <v>{
+    "structure":"My greatest weakness is _______.",
+    "main phrase":"lack of English skills",
+    "optional phrase 1":"lack of flexibility",
+    "optional phrase 2":"lack of confidence"
+}</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <v>[
+  {
+    "description": "TRẢ LỜI THEO TRANH GỢI Ý",
+    "sentence_en": "My greatest weakness is lack of English skills.",
+    "sentence_hide": "__ ________ ________ __ ____ __ _______ ______ ."
+  },
+  {
+    "description": "TRẢ LỜI THEO TRANH GỢI Ý",
+    "sentence_en": "My greatest weakness is lack of flexibility.",
+    "sentence_hide": "__ ________ ________ __ ____ __ ___________ ."
+  },
+  {
+    "description": "TRẢ LỜI THEO TRANH GỢI Ý",
+    "sentence_en": "My greatest weakness is lack of confidence.",
+    "sentence_hide": "__ ________ ________ __ ____ __ __________ ."
+  }
+]</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <v>You are provided with a question, structure, and three phrases.
+Instruction:
+sentence_en: Create an English sentence by replacing the phrase in the structure.
+sentence_hide: Blank out the entire sentence_en.
+**Important**: In each `sentence_hide` field, ensure the length of underscores (`_____`) matches the number of characters of the hidden word(s).
+Response JSON format (JSON not include other characters such as ```JSON)
+Example Input:
+Structure: "My greatest weakness is lack of _______."
+Phrases: "English skills", "flexibility", "confidence"
+Ouptu example: 
+[
+  {
+    ""description"": ""TRẢ LỜI THEO TRANH GỢI Ý"",
+    ""sentence_en"": ""My greatest weakness is lack of English skills."",
+    ""sentence_hide"": ""__ ________ ________ __ ____ __ _______ ______ .""
+  },
+  {
+    ""description"": ""TRẢ LỜI THEO TRANH GỢI Ý"",
+    ""sentence_en"": ""My greatest weakness is lack of flexibility."",
+    ""sentence_hide"": ""__ ________ ________ __ ____ __ ___________ .""
+  },
+  {
+    ""description"": ""TRẢ LỜI THEO TRANH GỢI Ý"",
+    ""sentence_en"": ""My greatest weakness is lack of confidence."",
+    ""sentence_hide"": ""__ ________ ________ __ ____ __ __________ .""
+  }
+]</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <v>I’ll follow up with you ________
+next week
+tomorrow 
+afternoonon Wednesday</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>

</xml_diff>

<commit_message>
deploy1.3_Conver_Prompt2Prompt+LogicCode. SIÊU BUG: QUÊN KO CHUYỂN config ở các file CALLAPI từ production -> sang development nên CODE SỬA HOÀI MÀ KO THẤY ĐƯỢC THAY ĐỔI,
</commit_message>
<xml_diff>
--- a/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
+++ b/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
@@ -102,13 +102,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD5F6F2"/>
+        <fgColor rgb="FFFFF5EB"/>
         <bgColor/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF5EB"/>
+        <fgColor rgb="FFD5F6F2"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -173,10 +173,10 @@
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -528,47 +528,49 @@
   </cols>
   <sheetData>
     <row customHeight="true" ht="40" r="1">
-      <c r="A1" s="5" t="str">
+      <c r="A1" s="3" t="str">
         <v>Công việc</v>
       </c>
-      <c r="B1" s="5" t="str">
+      <c r="B1" s="3" t="str">
         <v>Input</v>
       </c>
-      <c r="C1" s="5" t="str">
+      <c r="C1" s="3" t="str">
         <v>Output</v>
       </c>
-      <c r="D1" s="5" t="str">
+      <c r="D1" s="3" t="str">
         <v>Tham khảo</v>
       </c>
-      <c r="E1" s="5" t="str">
+      <c r="E1" s="3" t="str">
         <v>Prompt của a Hoàng</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3" t="str">
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="str">
         <v>input raw - từ Excel</v>
       </c>
-      <c r="H1" s="3" t="str">
+      <c r="H1" s="4" t="str">
         <v>output raw - từ Excel</v>
       </c>
-      <c r="I1" s="3" t="str">
+      <c r="I1" s="4" t="str">
         <v>prompt Cường</v>
       </c>
-      <c r="J1" s="3" t="str">
+      <c r="J1" s="4" t="str">
         <v>user_input - THOẢI MÁI, KO CẦN THEO JSON</v>
       </c>
-      <c r="K1" s="3" t="str">
+      <c r="K1" s="4" t="str">
         <v>output</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5" t="str">
+        <v>Prompt and Logic</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row customHeight="true" ht="113" r="2">
       <c r="A2" s="1"/>
@@ -679,7 +681,7 @@
    - Use `answer_1` as the exact `MAIN PHRASE` or `OTHER PHRASE`.
    - Provide alternatives for `answer_2` and `answer_3` with phrases close in meaning but incorrect.
 2. For each incorrect answer:
-   - Give a description explaining why it is incorrect, highlighting incorrect words with `&lt;r&gt;...&lt;/r&gt;` tags.
+   - Give a short description explaining why it is incorrect, highlighting incorrect words with `&lt;r&gt;...&lt;/r&gt;` tags.
 **Response Format:** Output only in JSON format with no extra characters  (such as ```Json) .
 **Example Input:**  
 - Cấu trúc: I'm the ______ from ABC Company.
@@ -692,19 +694,18 @@
         "answer_1": "Sales representative",
         "answer_2": "Business representative",
         "answer_3": "Sales agent",
-        "answer_2_description": "&lt;r&gt;Business representative&lt;/r&gt; không hoàn toàn đúng vì 'Business representative' thường mang nghĩa rộng hơn 'Đại diện kinh doanh', không chuyên biệt cho mảng bán hàng.",
-        "answer_3_description": "&lt;r&gt;Sales agent&lt;/r&gt; không hoàn toàn chính xác vì 'Sales agent' thường được dùng cho vai trò đại diện bán hàng theo hợp đồng, không bao hàm toàn bộ công việc của một 'Sales representative'."
+        "answer_2_description": "&lt;r&gt;Business representative&lt;/r&gt; rộng hơn 'Đại diện kinh doanh'.",
+        "answer_3_description": "&lt;r&gt;Sales agent&lt;/r&gt; thường là vai trò hợp đồng, không bao hàm đầy đủ trách nhiệm của 'Sales representative'."
     },
     {
         "sentence": "I'm the &lt;g&gt;Giám đốc kinh doanh&lt;/g&gt; from ABC Company.",
         "answer_1": "Sales director",
         "answer_2": "Sales manager",
         "answer_3": "Commercial director",
-        "answer_2_description": "&lt;r&gt;Sales manager&lt;/r&gt; không hoàn toàn đúng vì 'Sales manager' mang nghĩa là 'Quản lý kinh doanh' thay vì 'Giám đốc kinh doanh', thể hiện cấp bậc thấp hơn trong cấu trúc công ty.",
-        "answer_3_description": "&lt;r&gt;Commercial director&lt;/r&gt; không chính xác vì 'Commercial director' quản lý các hoạt động thương mại nói chung, không chuyên biệt về kinh doanh hoặc bán hàng."
+        "answer_2_description": "&lt;r&gt;Sales manager&lt;/r&gt; là quản lý, không phải giám đốc.",
+        "answer_3_description": "&lt;r&gt;Commercial director&lt;/r&gt; liên quan đến hoạt động thương mại, không chuyên về kinh doanh."
     }
-]
-</v>
+]</v>
       </c>
       <c r="J4" s="2" t="str" xml:space="preserve">
         <v> { 
@@ -796,7 +797,7 @@
     {
         "sentence_en": "Our team of _____ specialists is here to help",
         "sentence_vi": "Đội ngũ chuyên gia _____ của chúng tôi sẵn sàng hỗ trợ",
-        "ipa": "/ˈaʊər tiːm əv _____ ˈspɛʃəlɪsts ɪz hɪər tuː hɛlp/"
+        "ipa": "/ˈaʊər tiːm əv ____ ˈspɛʃəlɪsts ɪz hɪər tuː hɛlp/"
     },
     {
         "sentence_en": "healthcare specialists",
@@ -1029,7 +1030,35 @@
 ]</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1" t="str">
+        <v>
+---
+You are an expert at creating English exercise content.
+You will be given a `question`, a `structure`, and `3 phrases`.
+**Response JSON Format:**
+```json
+{
+  "question": {
+    "question": "What position are you applying for?",
+    "question_vn": "Bạn đang ứng tuyển vị trí nào?"
+  },
+  "sentence": [
+    {
+      "sentence": "I am applying for the ________ position.",
+      "sentence_vn": "Tôi đang ứng tuyển vị trí ________."
+    },
+    {
+      "sentence": "I would like to be a part of the ________ team.",
+      "sentence_vn": "Tôi muốn trở thành một phần của đội ngũ ________."
+    },
+    {
+      "sentence": "My goal is to become a ________ in this company.",
+      "sentence_vn": "Mục tiêu của tôi là trở thành một ________ trong công ty này."
+    }
+  ]
+}
+```</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1110,7 +1139,9 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1" t="str">
+        <v>Prompt cũ + Logic thay thế toàn bộ ký tự của  `sentence_hide` thành _</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>

</xml_diff>

<commit_message>
INIT Tracking Edit/Del Database OR FULL DATABASE
+ update thêm 1 chút phần Learning Meaning - cho oupput desctiption trả ra cố định format <r> ... </r> mang nghĩa ... nên sai so với yêu cầu đề bài
</commit_message>
<xml_diff>
--- a/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
+++ b/1_BuildWeb/ContentAppTheCoach/Requirements/Prompting.xlsx
@@ -34,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -44,6 +44,104 @@
     </font>
     <font>
       <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF1F2329"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF202123"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -80,8 +178,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none">
         <fgColor/>
@@ -96,7 +202,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB8C0BF"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFD5F6F2"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF04B49C"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2EA121"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF04B49C"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -113,7 +243,112 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="21">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -160,24 +395,69 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="7" fillId="0" fontId="7" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="9" fillId="0" fontId="9" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="10" fillId="3" fontId="10" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="11" fillId="4" fontId="11" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="12" fillId="0" fontId="12" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="13" fillId="0" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="14" fillId="5" fontId="14" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="15" fillId="0" fontId="15" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="16" fillId="6" fontId="16" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="17" fillId="0" fontId="17" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="18" fillId="7" fontId="18" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="19" fillId="8" fontId="19" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="20" fillId="0" fontId="20" numFmtId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,6 +474,47 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1666875</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>704850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2" descr="oFrEip"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="false"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect"/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="false" fPrintsWithSheet="true"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,7 +820,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="true" tabSelected="true" workbookViewId="0">
-      <pane state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="19"/>
@@ -521,59 +842,77 @@
     <col collapsed="false" customWidth="true" hidden="false" max="15" min="15" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="16" min="16" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" max="17" min="17" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="18" min="18" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="19" min="19" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="20" min="20" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="18" min="18" style="0" width="36"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="19" min="19" style="0" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="20" min="20" style="0" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" max="21" min="21" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="22" min="22" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="23" min="23" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="24" min="24" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="25" min="25" style="0" width="22"/>
   </cols>
   <sheetData>
     <row customHeight="true" ht="40" r="1">
-      <c r="A1" s="3" t="str">
+      <c r="A1" s="18" t="str">
         <v>Công việc</v>
       </c>
-      <c r="B1" s="3" t="str">
+      <c r="B1" s="18" t="str">
         <v>Input</v>
       </c>
-      <c r="C1" s="3" t="str">
+      <c r="C1" s="18" t="str">
         <v>Output</v>
       </c>
-      <c r="D1" s="3" t="str">
+      <c r="D1" s="18" t="str">
         <v>Tham khảo</v>
       </c>
-      <c r="E1" s="3" t="str">
+      <c r="E1" s="18" t="str">
         <v>Prompt của a Hoàng</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4" t="str">
+      <c r="F1" s="17"/>
+      <c r="G1" s="19" t="str">
         <v>input raw - từ Excel</v>
       </c>
-      <c r="H1" s="4" t="str">
+      <c r="H1" s="19" t="str">
         <v>output raw - từ Excel</v>
       </c>
-      <c r="I1" s="4" t="str">
+      <c r="I1" s="19" t="str">
         <v>prompt Cường</v>
       </c>
-      <c r="J1" s="4" t="str">
+      <c r="J1" s="19" t="str">
         <v>user_input - THOẢI MÁI, KO CẦN THEO JSON</v>
       </c>
-      <c r="K1" s="4" t="str">
+      <c r="K1" s="19" t="str">
         <v>output</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="str">
+      <c r="L1" s="17"/>
+      <c r="M1" s="17" t="str">
         <v>Prompt and Logic</v>
       </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-    </row>
-    <row customHeight="true" ht="113" r="2">
-      <c r="A2" s="1"/>
+      <c r="N1" s="17" t="str">
+        <v>Input cũ thui</v>
+      </c>
+      <c r="O1" s="17" t="str">
+        <v>Output mới</v>
+      </c>
+      <c r="P1" s="20" t="str">
+        <v>Số token input</v>
+      </c>
+      <c r="Q1" s="20" t="str">
+        <v>Số token output</v>
+      </c>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+    </row>
+    <row customHeight="true" ht="58" r="2">
+      <c r="A2" s="1" t="str">
+        <v>Draft học liệu (2 câu)</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="str">
         <v>[
@@ -594,55 +933,98 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="11" t="str">
+        <v>Generate ${questionCount} English lesson questions on "${topic}" at ${level} level, 
+and MUST meet the following additional requirements: ${extraRequirements}. 
+Instructions: 
+{
+  "question": "Question text",
+  "structure": "Answer format with blank (____), ONLY 1 blank for the answer",
+  "main phrase": "Key phrase to fit blank (no proper nouns and must be a phrase 1, 2, 3, 4 words)", 
+  "optional phrase 1": "Alternative phrase option 1 (no proper nouns and must be a phrase 1, 2, 3, 4 words)",
+  "optional phrase 2": "Alternative phrase option 2 (no proper nouns and must be a phrase 1, 2, 3, 4 words)",
+  "question-vi": "Vietnamese translation of question",
+  "structure-vi": "Vietnamese translation of structure",
+  "main phrase-vi": "Vietnamese translation of main phrase",
+  "optional phrase 1-vi": "Vietnamese translation of option 1",
+  "optional phrase 2-vi": "Vietnamese translation of option 2"
+}
+Example:
+{
+  "question": "Which company are you working for?",
+  "structure": "I'm the ____ from ABC Company.",
+  "main phrase": "Sales representative",
+  "optional phrase 1": "Sales director", 
+  "optional phrase 2": "Sales associate",
+  "question-vi": "Bạn đang làm việc cho công ty nào vậy?",
+  "structure-vi": "Tôi là ____ từ công ty ABC.",
+  "main phrase-vi": "Đại diện kinh doanh",
+  "optional phrase 1-vi": "Giám đốc kinh doanh",
+  "optional phrase 2-vi": "Nhân viên bán hàng"
+}</v>
+      </c>
+      <c r="J2" s="11" t="str">
+        <v>topic: đi học về
+question: 2</v>
+      </c>
+      <c r="K2" s="11" t="str">
+        <v>Here are 2 English lesson questions on the topic "going to school" at an intermediate level:
+1. {
+ "question": "What time do you usually leave for school?",
+ "structure": "I usually leave for school at ____.",
+ "main phrase": "seven o'clock",
+ "optional phrase 1": "eight o'clock", 
+ "optional phrase 2": "six thirty",
+ "question-vi": "Bạn thường rời nhà đi học lúc mấy giờ?",
+ "structure-vi": "Tôi thường rời nhà đi học lúc ____.",
+ "main phrase-vi": "bảy giờ",
+ "optional phrase 1-vi": "tám giờ",
+ "optional phrase 2-vi": "sáu giờ ba mươi"
+}
+2. {
+ "question": "How do you get to school?",
+ "structure": "I get to school by ____.",
+ "main phrase": "bus",
+ "optional phrase 1": "bicycle", 
+ "optional phrase 2": "walking",
+ "question-vi": "Bạn đi học bằng phương tiện gì?",
+ "structure-vi": "Tôi đi học bằng ____.",
+ "main phrase-vi": "xe buýt",
+ "optional phrase 1-vi": "xe đạp",
+ "optional phrase 2-vi": "đi bộ"
+}</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
+      <c r="P2" s="12">
+        <v>386</v>
+      </c>
+      <c r="Q2" s="12">
+        <v>273</v>
+      </c>
+      <c r="R2" s="13"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="3">
-      <c r="A3" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row customHeight="true" ht="58" r="3">
+      <c r="A3" s="1" t="str" xml:space="preserve">
+        <v>Dạng 1: Learning Meaning Exercise </v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="4">
-      <c r="A4" s="1" t="str" xml:space="preserve">
-        <v>Dạng 1: Learning Meaning Exercise </v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2" t="str" xml:space="preserve">
+      <c r="G3" s="1" t="str" xml:space="preserve">
         <v>Câu hỏi
 Cấu trúc
 Cụm thông tin
@@ -655,7 +1037,7 @@
 Sales associate
  </v>
       </c>
-      <c r="H4" s="2" t="str" xml:space="preserve">
+      <c r="H3" s="1" t="str" xml:space="preserve">
         <v>description
 sentence
 answer_1
@@ -673,7 +1055,7 @@
 Sales Associate
  </v>
       </c>
-      <c r="I4" s="2" t="str">
+      <c r="I3" s="11" t="str">
         <v>**Prompt:**  
 You are an expert at creating English exercise content. You will receive `CẤU TRÚC`, `MAIN PHRASE`, and `OTHER PHRASE` inputs from the user.
 **Instructions:**  
@@ -707,14 +1089,14 @@
     }
 ]</v>
       </c>
-      <c r="J4" s="2" t="str" xml:space="preserve">
+      <c r="J3" s="11" t="str" xml:space="preserve">
         <v> { 
  "structure": "I'm the ______ from ABC Company.", 
 "mainPhrase": "Sales representative", 
  "optionalPhrase": "Sales director" 
 }</v>
       </c>
-      <c r="K4" s="2" t="str">
+      <c r="K3" s="11" t="str">
         <v>[
  {
  "sentence": "I'm the &lt;g&gt;Đại diện kinh doanh&lt;/g&gt; from ABC Company.",
@@ -734,25 +1116,37 @@
  }
 ]</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2" t="str" xml:space="preserve">
+      <c r="L3" s="1"/>
+      <c r="M3" s="14" t="str">
+        <v>MÀU XANH LÁ CÂY LÀ PROMPT ĐANG DÙNG</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="12">
+        <v>421</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>308</v>
+      </c>
+      <c r="R3" s="13"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row customHeight="true" ht="58" r="4">
+      <c r="A4" s="1" t="str">
+        <v>Dạng 2: Learning Card</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="str" xml:space="preserve">
         <v>Main phrase
 Optional phrase
 Sales representative
@@ -760,7 +1154,7 @@
 Sales associate
  </v>
       </c>
-      <c r="H5" s="2" t="str" xml:space="preserve">
+      <c r="H4" s="1" t="str" xml:space="preserve">
         <v>description
 sentence_en
 sentence_vi
@@ -779,7 +1173,7 @@
 /seɪlz əˈsoʊʃiət/
  </v>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="I4" s="11" t="str">
         <v>You are an English exercise content expert. Given structure_en, main_phrase, and up to two optional_phrases, create a JSON array with:
 - sentence_en: English sentence
 - sentence_vi: Vietnamese translation
@@ -816,14 +1210,14 @@
     }
 ]</v>
       </c>
-      <c r="J5" s="2" t="str" xml:space="preserve">
+      <c r="J4" s="11" t="str" xml:space="preserve">
         <v>We're a _____
 promising start-up
 leading firm
 pioneer company 
  </v>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K4" s="11" t="str">
         <v>[
   {
     "sentence_en": "Promising start-up",
@@ -842,25 +1236,35 @@
   }
 ]</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2" t="str" xml:space="preserve">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="12">
+        <v>369</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>161</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row customHeight="true" ht="58" r="5">
+      <c r="A5" s="1" t="str">
+        <v>Dạng 3: Learning Flexible</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="5" t="str" xml:space="preserve">
         <v>Câu hỏi
 Cấu trúc
 Cụm thông tin
@@ -873,7 +1277,7 @@
 Sales associate
  </v>
       </c>
-      <c r="H6" s="2" t="str" xml:space="preserve">
+      <c r="H5" s="5" t="str" xml:space="preserve">
         <v>sentence_hide
 sentence_en
 sentence_vi
@@ -903,7 +1307,7 @@
 Bạn đang làm việc cho công ty nào vậy?
  </v>
       </c>
-      <c r="I6" s="2" t="str">
+      <c r="I5" s="5" t="str">
         <v>
 **Prompt:**
 You are an expert at creating English exercise content. Based on the given structure, generate a JSON response with various English sentences, where specific words are hidden to create fill-in-the-blank exercises. Translate each sentence into Vietnamese.
@@ -971,13 +1375,13 @@
     }
 ]</v>
       </c>
-      <c r="J6" s="2" t="str">
+      <c r="J5" s="5" t="str">
         <v>I’ll follow up with you ________
 next week
 tomorrow 
 afternoonon Wednesday</v>
       </c>
-      <c r="K6" s="2" t="str">
+      <c r="K5" s="5" t="str">
         <v>[
   {
     "description": "Hãy nghe mình nói và đọc lại",
@@ -1029,53 +1433,89 @@
   }
 ]</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1" t="str">
-        <v>
----
-You are an expert at creating English exercise content.
-You will be given a `question`, a `structure`, and `3 phrases`.
-**Response JSON Format:**
-```json
+      <c r="L5" s="1"/>
+      <c r="M5" s="16" t="str">
+        <v>You are an expert at creating English exercise content. 
+You sẽ được cung cấp 1 'question', 1 'structure', and 3 'phrases'. 
+Ví dụ input:
+{
+  "question": "Which company are you working for?",
+  "structure": "I'm the ______ from ABC Company.",
+  "phrases": ["Sales representative", "Sales director", "Sales associate"]
+}
+Response format:
 {
   "question": {
-    "question": "What position are you applying for?",
-    "question_vn": "Bạn đang ứng tuyển vị trí nào?"
+    "question": "Which company are you working for?",
+    "question_vn": "Bạn đang làm việc cho công ty nào?"
   },
   "sentence": [
     {
-      "sentence": "I am applying for the ________ position.",
-      "sentence_vn": "Tôi đang ứng tuyển vị trí ________."
+      "sentence": "I'm the Sales representative from ABC Company.",
+      "sentence_vn": "Tôi là đại diện kinh doanh của công ty ABC."
     },
     {
-      "sentence": "I would like to be a part of the ________ team.",
-      "sentence_vn": "Tôi muốn trở thành một phần của đội ngũ ________."
+      "sentence": "I'm the Sales director from ABC Company.",
+      "sentence_vn": "Tôi là giám đốc kinh doanh của công ty ABC."
     },
     {
-      "sentence": "My goal is to become a ________ in this company.",
-      "sentence_vn": "Mục tiêu của tôi là trở thành một ________ trong công ty này."
+      "sentence": "I'm the Sales associate from ABC Company.",
+      "sentence_vn": "Tôi là nhân viên bán hàng của công ty ABC."
     }
   ]
-}
-```</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2" t="str">
+}</v>
+      </c>
+      <c r="N5" s="16" t="str" xml:space="preserve">
+        <v>Ko cần JSON
+ 1 'question', 1 'structure', and 3 'phrases'. </v>
+      </c>
+      <c r="O5" s="16" t="str">
+        <v>{
+  "question": {
+    "question": "Which company are you working for?",
+    "question_vn": "Bạn đang làm việc cho công ty nào?"
+  },
+  "sentence": [
+    {
+      "sentence": "I'm the Sales representative from ABC Company.",
+      "sentence_vn": "Tôi là đại diện kinh doanh của công ty ABC."
+    },
+    {
+      "sentence": "I'm the Sales director from ABC Company.",
+      "sentence_vn": "Tôi là giám đốc kinh doanh của công ty ABC."
+    },
+    {
+      "sentence": "I'm the Sales associate from ABC Company.",
+      "sentence_vn": "Tôi là nhân viên bán hàng của công ty ABC."
+    }
+  ]
+}</v>
+      </c>
+      <c r="P5" s="12">
+        <v>743</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>499</v>
+      </c>
+      <c r="R5" s="13"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row customHeight="true" ht="58" r="6">
+      <c r="A6" s="1" t="str">
+        <v>Dạng 4: Learning Q&amp;A</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5" t="str">
         <v>{
     "structure":"My greatest weakness is _______.",
     "main phrase":"lack of English skills",
@@ -1083,7 +1523,7 @@
     "optional phrase 2":"lack of confidence"
 }</v>
       </c>
-      <c r="H7" s="2" t="str">
+      <c r="H6" s="5" t="str">
         <v>[
   {
     "description": "TRẢ LỜI THEO TRANH GỢI Ý",
@@ -1102,7 +1542,7 @@
   }
 ]</v>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="I6" s="5" t="str">
         <v>You are provided with a question, structure, and three phrases.
 Instruction:
 sentence_en: Create an English sentence by replacing the phrase in the structure.
@@ -1131,94 +1571,176 @@
   }
 ]</v>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="J6" s="5" t="str">
         <v>I’ll follow up with you ________
 next week
 tomorrow 
 afternoonon Wednesday</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1" t="str">
+        <v>Full Logic</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <v>Full Logic</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <v>Full Logic</v>
+      </c>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="3"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row customHeight="true" ht="50" r="7">
+      <c r="A7" s="1" t="str">
+        <v>Tổng số token</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1" t="str">
-        <v>Prompt cũ + Logic thay thế toàn bộ ký tự của  `sentence_hide` thành _</v>
-      </c>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="P7" s="6">
+        <f>SUM(P2:P5)</f>
+      </c>
+      <c r="Q7" s="6">
+        <f>SUM(Q2:Q5)</f>
+      </c>
+      <c r="R7" s="6">
+        <f>SUM(P7:Q7)</f>
+      </c>
+      <c r="S7" s="15"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="8">
-      <c r="A8" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row customHeight="true" ht="48" r="8">
+      <c r="A8" s="1" t="str">
+        <v>Thành tiền ($)</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="O8" s="1" t="str">
+        <v>1 câu gen đủ cả draft và 4 dạng là 8k</v>
+      </c>
+      <c r="P8" s="6">
+        <f>P7*0.000075/1000</f>
+      </c>
+      <c r="Q8" s="6">
+        <f>0.0003/1000*Q7</f>
+      </c>
+      <c r="R8" s="6">
+        <f>SUM(P8:Q8)</f>
+      </c>
+      <c r="S8" s="15"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="9">
-      <c r="A9" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row customHeight="true" ht="45" r="9">
+      <c r="A9" s="1" t="str">
+        <v>Thành tiền (nghìn vnd) cho 2 câu học liệu</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+      <c r="O9" s="1" t="str">
+        <v>6 câu = 28k 1 lần gen học liệu</v>
+      </c>
+      <c r="P9" s="6">
+        <f>P8*25</f>
+      </c>
+      <c r="Q9" s="6">
+        <f>Q8*25</f>
+      </c>
+      <c r="R9" s="6">
+        <f>R8*25</f>
+      </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="10">
-      <c r="A10" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row customHeight="true" ht="52" r="10">
+      <c r="A10" s="8" t="str">
+        <v>Nhận xét</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="P10" s="7" t="str">
+        <v>Input không đổi</v>
+      </c>
+      <c r="Q10" s="6" t="str">
+        <v>Mỗi câu thêm sẽ thêm 0.004 nghìn</v>
+      </c>
+      <c r="R10" s="9" t="str">
+        <v>1 lần gen trung bình 6 câu sẽ mất 0.008 + 0.004*5 = 0.0028 nghìn</v>
+      </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="11">
       <c r="A11" s="1"/>
@@ -1236,12 +1758,16 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="12">
       <c r="A12" s="1"/>
@@ -1259,12 +1785,16 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="13">
       <c r="A13" s="1"/>
@@ -1282,12 +1812,16 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="14">
       <c r="A14" s="1"/>
@@ -1305,12 +1839,16 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="15">
       <c r="A15" s="1"/>
@@ -1328,12 +1866,16 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="16">
       <c r="A16" s="1"/>
@@ -1351,12 +1893,16 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="17">
       <c r="A17" s="1"/>
@@ -1374,12 +1920,16 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="18">
       <c r="A18" s="1"/>
@@ -1397,12 +1947,16 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="19">
       <c r="A19" s="1"/>
@@ -1420,12 +1974,16 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="20">
       <c r="A20" s="1"/>
@@ -1443,12 +2001,16 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="21">
       <c r="A21" s="1"/>
@@ -1466,12 +2028,16 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="22">
       <c r="A22" s="1"/>
@@ -1489,12 +2055,16 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="23">
       <c r="A23" s="1"/>
@@ -1512,12 +2082,16 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="24">
       <c r="A24" s="1"/>
@@ -1535,12 +2109,16 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="25">
       <c r="A25" s="1"/>
@@ -1558,12 +2136,16 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="26">
       <c r="A26" s="1"/>
@@ -1581,12 +2163,16 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="27">
       <c r="A27" s="1"/>
@@ -1604,12 +2190,16 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="28">
       <c r="A28" s="1"/>
@@ -1627,12 +2217,16 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="29">
       <c r="A29" s="1"/>
@@ -1650,12 +2244,16 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="30">
       <c r="A30" s="1"/>
@@ -1673,12 +2271,16 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="31">
       <c r="A31" s="1"/>
@@ -1696,12 +2298,16 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="32">
       <c r="A32" s="1"/>
@@ -1719,12 +2325,16 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="33">
       <c r="A33" s="1"/>
@@ -1742,12 +2352,16 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="34">
       <c r="A34" s="1"/>
@@ -1765,12 +2379,16 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="35">
       <c r="A35" s="1"/>
@@ -1788,12 +2406,16 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="36">
       <c r="A36" s="1"/>
@@ -1811,12 +2433,16 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="37">
       <c r="A37" s="1"/>
@@ -1834,12 +2460,16 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="38">
       <c r="A38" s="1"/>
@@ -1857,12 +2487,16 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="39">
       <c r="A39" s="1"/>
@@ -1880,12 +2514,16 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="40">
       <c r="A40" s="1"/>
@@ -1903,12 +2541,16 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="41">
       <c r="A41" s="1"/>
@@ -1926,12 +2568,16 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="42">
       <c r="A42" s="1"/>
@@ -1949,12 +2595,16 @@
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="43">
       <c r="A43" s="1"/>
@@ -1972,12 +2622,16 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="44">
       <c r="A44" s="1"/>
@@ -1995,12 +2649,16 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="45">
       <c r="A45" s="1"/>
@@ -2018,12 +2676,16 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="46">
       <c r="A46" s="1"/>
@@ -2041,12 +2703,16 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="47">
       <c r="A47" s="1"/>
@@ -2064,12 +2730,16 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="48">
       <c r="A48" s="1"/>
@@ -2087,12 +2757,16 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="49">
       <c r="A49" s="1"/>
@@ -2110,12 +2784,16 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="50">
       <c r="A50" s="1"/>
@@ -2133,12 +2811,16 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+      <c r="Y50" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="51">
       <c r="A51" s="1"/>
@@ -2156,12 +2838,16 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="52">
       <c r="A52" s="1"/>
@@ -2179,12 +2865,16 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="53">
       <c r="A53" s="1"/>
@@ -2202,12 +2892,16 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+      <c r="Y53" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="54">
       <c r="A54" s="1"/>
@@ -2225,12 +2919,16 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
+      <c r="P54" s="2"/>
+      <c r="Q54" s="2"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+      <c r="Y54" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="55">
       <c r="A55" s="1"/>
@@ -2248,12 +2946,16 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
+      <c r="P55" s="2"/>
+      <c r="Q55" s="2"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+      <c r="Y55" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="56">
       <c r="A56" s="1"/>
@@ -2271,12 +2973,16 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
+      <c r="P56" s="2"/>
+      <c r="Q56" s="2"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="57">
       <c r="A57" s="1"/>
@@ -2294,12 +3000,16 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="58">
       <c r="A58" s="1"/>
@@ -2317,12 +3027,16 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
+      <c r="P58" s="2"/>
+      <c r="Q58" s="2"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="59">
       <c r="A59" s="1"/>
@@ -2340,12 +3054,16 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
+      <c r="P59" s="2"/>
+      <c r="Q59" s="2"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="60">
       <c r="A60" s="1"/>
@@ -2363,12 +3081,16 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
+      <c r="P60" s="2"/>
+      <c r="Q60" s="2"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="61">
       <c r="A61" s="1"/>
@@ -2386,12 +3108,16 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2"/>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="62">
       <c r="A62" s="1"/>
@@ -2409,12 +3135,16 @@
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="63">
       <c r="A63" s="1"/>
@@ -2432,12 +3162,16 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="64">
       <c r="A64" s="1"/>
@@ -2455,12 +3189,16 @@
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+      <c r="Y64" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="65">
       <c r="A65" s="1"/>
@@ -2478,12 +3216,16 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+      <c r="Y65" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="66">
       <c r="A66" s="1"/>
@@ -2501,12 +3243,16 @@
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+      <c r="Y66" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="67">
       <c r="A67" s="1"/>
@@ -2524,12 +3270,16 @@
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+      <c r="Y67" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="68">
       <c r="A68" s="1"/>
@@ -2547,12 +3297,16 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="Y68" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="69">
       <c r="A69" s="1"/>
@@ -2570,12 +3324,16 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="2"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="70">
       <c r="A70" s="1"/>
@@ -2593,12 +3351,16 @@
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="71">
       <c r="A71" s="1"/>
@@ -2616,12 +3378,16 @@
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
-      <c r="P71" s="1"/>
-      <c r="Q71" s="1"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="72">
       <c r="A72" s="1"/>
@@ -2639,12 +3405,16 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="73">
       <c r="A73" s="1"/>
@@ -2662,12 +3432,16 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
-      <c r="P73" s="1"/>
-      <c r="Q73" s="1"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+      <c r="Y73" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="74">
       <c r="A74" s="1"/>
@@ -2685,12 +3459,16 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
       <c r="R74" s="1"/>
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+      <c r="Y74" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="75">
       <c r="A75" s="1"/>
@@ -2708,12 +3486,16 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
-      <c r="P75" s="1"/>
-      <c r="Q75" s="1"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
       <c r="R75" s="1"/>
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="76">
       <c r="A76" s="1"/>
@@ -2731,12 +3513,16 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
-      <c r="P76" s="1"/>
-      <c r="Q76" s="1"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
       <c r="R76" s="1"/>
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+      <c r="Y76" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="77">
       <c r="A77" s="1"/>
@@ -2754,12 +3540,16 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+      <c r="Y77" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="78">
       <c r="A78" s="1"/>
@@ -2777,12 +3567,16 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
-      <c r="P78" s="1"/>
-      <c r="Q78" s="1"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+      <c r="Y78" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="79">
       <c r="A79" s="1"/>
@@ -2800,12 +3594,16 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
-      <c r="P79" s="1"/>
-      <c r="Q79" s="1"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+      <c r="Y79" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="80">
       <c r="A80" s="1"/>
@@ -2823,12 +3621,16 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="81">
       <c r="A81" s="1"/>
@@ -2846,12 +3648,16 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
-      <c r="P81" s="1"/>
-      <c r="Q81" s="1"/>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+      <c r="Y81" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="82">
       <c r="A82" s="1"/>
@@ -2869,12 +3675,16 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
-      <c r="P82" s="1"/>
-      <c r="Q82" s="1"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+      <c r="Y82" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="83">
       <c r="A83" s="1"/>
@@ -2892,12 +3702,16 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
-      <c r="P83" s="1"/>
-      <c r="Q83" s="1"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+      <c r="Y83" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="84">
       <c r="A84" s="1"/>
@@ -2915,12 +3729,16 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
-      <c r="P84" s="1"/>
-      <c r="Q84" s="1"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+      <c r="Y84" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="85">
       <c r="A85" s="1"/>
@@ -2938,12 +3756,16 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
-      <c r="P85" s="1"/>
-      <c r="Q85" s="1"/>
+      <c r="P85" s="2"/>
+      <c r="Q85" s="2"/>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+      <c r="Y85" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="86">
       <c r="A86" s="1"/>
@@ -2961,12 +3783,16 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
+      <c r="P86" s="2"/>
+      <c r="Q86" s="2"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+      <c r="Y86" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="87">
       <c r="A87" s="1"/>
@@ -2984,12 +3810,16 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="1"/>
-      <c r="Q87" s="1"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="88">
       <c r="A88" s="1"/>
@@ -3007,12 +3837,16 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
-      <c r="P88" s="1"/>
-      <c r="Q88" s="1"/>
+      <c r="P88" s="2"/>
+      <c r="Q88" s="2"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="89">
       <c r="A89" s="1"/>
@@ -3030,12 +3864,16 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="1"/>
-      <c r="Q89" s="1"/>
+      <c r="P89" s="2"/>
+      <c r="Q89" s="2"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+      <c r="Y89" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="90">
       <c r="A90" s="1"/>
@@ -3053,12 +3891,16 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+      <c r="Y90" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="91">
       <c r="A91" s="1"/>
@@ -3076,12 +3918,16 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
-      <c r="P91" s="1"/>
-      <c r="Q91" s="1"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="2"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+      <c r="Y91" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="92">
       <c r="A92" s="1"/>
@@ -3099,12 +3945,16 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+      <c r="Y92" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="93">
       <c r="A93" s="1"/>
@@ -3122,12 +3972,16 @@
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
-      <c r="P93" s="1"/>
-      <c r="Q93" s="1"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
       <c r="R93" s="1"/>
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+      <c r="Y93" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="94">
       <c r="A94" s="1"/>
@@ -3145,12 +3999,16 @@
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
-      <c r="P94" s="1"/>
-      <c r="Q94" s="1"/>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="95">
       <c r="A95" s="1"/>
@@ -3168,12 +4026,16 @@
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
-      <c r="P95" s="1"/>
-      <c r="Q95" s="1"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="96">
       <c r="A96" s="1"/>
@@ -3191,12 +4053,16 @@
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
-      <c r="P96" s="1"/>
-      <c r="Q96" s="1"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+      <c r="Y96" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="97">
       <c r="A97" s="1"/>
@@ -3214,12 +4080,16 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
-      <c r="P97" s="1"/>
-      <c r="Q97" s="1"/>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="2"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+      <c r="Y97" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="98">
       <c r="A98" s="1"/>
@@ -3237,12 +4107,16 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
+      <c r="V98" s="1"/>
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+      <c r="Y98" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="99">
       <c r="A99" s="1"/>
@@ -3260,12 +4134,16 @@
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
-      <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
+      <c r="P99" s="2"/>
+      <c r="Q99" s="2"/>
       <c r="R99" s="1"/>
       <c r="S99" s="1"/>
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
+      <c r="V99" s="1"/>
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+      <c r="Y99" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="100">
       <c r="A100" s="1"/>
@@ -3283,12 +4161,16 @@
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
-      <c r="P100" s="1"/>
-      <c r="Q100" s="1"/>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="2"/>
       <c r="R100" s="1"/>
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
+      <c r="V100" s="1"/>
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+      <c r="Y100" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="101">
       <c r="A101" s="1"/>
@@ -3306,12 +4188,16 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
       <c r="R101" s="1"/>
       <c r="S101" s="1"/>
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="102">
       <c r="A102" s="1"/>
@@ -3329,12 +4215,16 @@
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
+      <c r="V102" s="1"/>
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+      <c r="Y102" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="103">
       <c r="A103" s="1"/>
@@ -3352,12 +4242,16 @@
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
+      <c r="V103" s="1"/>
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+      <c r="Y103" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="104">
       <c r="A104" s="1"/>
@@ -3375,12 +4269,16 @@
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
-      <c r="P104" s="1"/>
-      <c r="Q104" s="1"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+      <c r="Y104" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="105">
       <c r="A105" s="1"/>
@@ -3398,12 +4296,16 @@
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
+      <c r="P105" s="2"/>
+      <c r="Q105" s="2"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="106">
       <c r="A106" s="1"/>
@@ -3421,12 +4323,16 @@
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
-      <c r="P106" s="1"/>
-      <c r="Q106" s="1"/>
+      <c r="P106" s="2"/>
+      <c r="Q106" s="2"/>
       <c r="R106" s="1"/>
       <c r="S106" s="1"/>
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+      <c r="Y106" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="107">
       <c r="A107" s="1"/>
@@ -3444,12 +4350,16 @@
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
-      <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
+      <c r="P107" s="2"/>
+      <c r="Q107" s="2"/>
       <c r="R107" s="1"/>
       <c r="S107" s="1"/>
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
+      <c r="V107" s="1"/>
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
+      <c r="Y107" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="108">
       <c r="A108" s="1"/>
@@ -3467,12 +4377,16 @@
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
-      <c r="P108" s="1"/>
-      <c r="Q108" s="1"/>
+      <c r="P108" s="2"/>
+      <c r="Q108" s="2"/>
       <c r="R108" s="1"/>
       <c r="S108" s="1"/>
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
+      <c r="V108" s="1"/>
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
+      <c r="Y108" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="109">
       <c r="A109" s="1"/>
@@ -3490,12 +4404,16 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
-      <c r="P109" s="1"/>
-      <c r="Q109" s="1"/>
+      <c r="P109" s="2"/>
+      <c r="Q109" s="2"/>
       <c r="R109" s="1"/>
       <c r="S109" s="1"/>
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+      <c r="Y109" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="110">
       <c r="A110" s="1"/>
@@ -3513,12 +4431,16 @@
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
+      <c r="P110" s="2"/>
+      <c r="Q110" s="2"/>
       <c r="R110" s="1"/>
       <c r="S110" s="1"/>
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+      <c r="Y110" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="111">
       <c r="A111" s="1"/>
@@ -3536,12 +4458,16 @@
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
-      <c r="P111" s="1"/>
-      <c r="Q111" s="1"/>
+      <c r="P111" s="2"/>
+      <c r="Q111" s="2"/>
       <c r="R111" s="1"/>
       <c r="S111" s="1"/>
       <c r="T111" s="1"/>
       <c r="U111" s="1"/>
+      <c r="V111" s="1"/>
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
+      <c r="Y111" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="112">
       <c r="A112" s="1"/>
@@ -3559,12 +4485,16 @@
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
       <c r="R112" s="1"/>
       <c r="S112" s="1"/>
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
+      <c r="V112" s="1"/>
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+      <c r="Y112" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="113">
       <c r="A113" s="1"/>
@@ -3582,12 +4512,16 @@
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
-      <c r="P113" s="1"/>
-      <c r="Q113" s="1"/>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
       <c r="R113" s="1"/>
       <c r="S113" s="1"/>
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
+      <c r="V113" s="1"/>
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+      <c r="Y113" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="114">
       <c r="A114" s="1"/>
@@ -3605,12 +4539,16 @@
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
-      <c r="P114" s="1"/>
-      <c r="Q114" s="1"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
       <c r="R114" s="1"/>
       <c r="S114" s="1"/>
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
+      <c r="V114" s="1"/>
+      <c r="W114" s="1"/>
+      <c r="X114" s="1"/>
+      <c r="Y114" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="115">
       <c r="A115" s="1"/>
@@ -3628,12 +4566,16 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
-      <c r="P115" s="1"/>
-      <c r="Q115" s="1"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
+      <c r="V115" s="1"/>
+      <c r="W115" s="1"/>
+      <c r="X115" s="1"/>
+      <c r="Y115" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="116">
       <c r="A116" s="1"/>
@@ -3651,12 +4593,16 @@
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
-      <c r="P116" s="1"/>
-      <c r="Q116" s="1"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
       <c r="R116" s="1"/>
       <c r="S116" s="1"/>
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
+      <c r="V116" s="1"/>
+      <c r="W116" s="1"/>
+      <c r="X116" s="1"/>
+      <c r="Y116" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="117">
       <c r="A117" s="1"/>
@@ -3674,12 +4620,16 @@
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
       <c r="O117" s="1"/>
-      <c r="P117" s="1"/>
-      <c r="Q117" s="1"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
       <c r="R117" s="1"/>
       <c r="S117" s="1"/>
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
+      <c r="V117" s="1"/>
+      <c r="W117" s="1"/>
+      <c r="X117" s="1"/>
+      <c r="Y117" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="118">
       <c r="A118" s="1"/>
@@ -3697,12 +4647,16 @@
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
-      <c r="P118" s="1"/>
-      <c r="Q118" s="1"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
       <c r="R118" s="1"/>
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
+      <c r="V118" s="1"/>
+      <c r="W118" s="1"/>
+      <c r="X118" s="1"/>
+      <c r="Y118" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="119">
       <c r="A119" s="1"/>
@@ -3720,12 +4674,16 @@
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
       <c r="O119" s="1"/>
-      <c r="P119" s="1"/>
-      <c r="Q119" s="1"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
       <c r="R119" s="1"/>
       <c r="S119" s="1"/>
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
+      <c r="V119" s="1"/>
+      <c r="W119" s="1"/>
+      <c r="X119" s="1"/>
+      <c r="Y119" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="120">
       <c r="A120" s="1"/>
@@ -3743,12 +4701,16 @@
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
       <c r="O120" s="1"/>
-      <c r="P120" s="1"/>
-      <c r="Q120" s="1"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
       <c r="R120" s="1"/>
       <c r="S120" s="1"/>
       <c r="T120" s="1"/>
       <c r="U120" s="1"/>
+      <c r="V120" s="1"/>
+      <c r="W120" s="1"/>
+      <c r="X120" s="1"/>
+      <c r="Y120" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="121">
       <c r="A121" s="1"/>
@@ -3766,12 +4728,16 @@
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
-      <c r="P121" s="1"/>
-      <c r="Q121" s="1"/>
+      <c r="P121" s="2"/>
+      <c r="Q121" s="2"/>
       <c r="R121" s="1"/>
       <c r="S121" s="1"/>
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
+      <c r="V121" s="1"/>
+      <c r="W121" s="1"/>
+      <c r="X121" s="1"/>
+      <c r="Y121" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="122">
       <c r="A122" s="1"/>
@@ -3789,12 +4755,16 @@
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
       <c r="O122" s="1"/>
-      <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
+      <c r="V122" s="1"/>
+      <c r="W122" s="1"/>
+      <c r="X122" s="1"/>
+      <c r="Y122" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="123">
       <c r="A123" s="1"/>
@@ -3812,12 +4782,16 @@
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
       <c r="O123" s="1"/>
-      <c r="P123" s="1"/>
-      <c r="Q123" s="1"/>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
       <c r="R123" s="1"/>
       <c r="S123" s="1"/>
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
+      <c r="V123" s="1"/>
+      <c r="W123" s="1"/>
+      <c r="X123" s="1"/>
+      <c r="Y123" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="124">
       <c r="A124" s="1"/>
@@ -3835,12 +4809,16 @@
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
-      <c r="P124" s="1"/>
-      <c r="Q124" s="1"/>
+      <c r="P124" s="2"/>
+      <c r="Q124" s="2"/>
       <c r="R124" s="1"/>
       <c r="S124" s="1"/>
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
+      <c r="V124" s="1"/>
+      <c r="W124" s="1"/>
+      <c r="X124" s="1"/>
+      <c r="Y124" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="125">
       <c r="A125" s="1"/>
@@ -3858,12 +4836,16 @@
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
-      <c r="P125" s="1"/>
-      <c r="Q125" s="1"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
+      <c r="V125" s="1"/>
+      <c r="W125" s="1"/>
+      <c r="X125" s="1"/>
+      <c r="Y125" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="126">
       <c r="A126" s="1"/>
@@ -3881,12 +4863,16 @@
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
-      <c r="P126" s="1"/>
-      <c r="Q126" s="1"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
       <c r="T126" s="1"/>
       <c r="U126" s="1"/>
+      <c r="V126" s="1"/>
+      <c r="W126" s="1"/>
+      <c r="X126" s="1"/>
+      <c r="Y126" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="127">
       <c r="A127" s="1"/>
@@ -3904,12 +4890,16 @@
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
-      <c r="P127" s="1"/>
-      <c r="Q127" s="1"/>
+      <c r="P127" s="2"/>
+      <c r="Q127" s="2"/>
       <c r="R127" s="1"/>
       <c r="S127" s="1"/>
       <c r="T127" s="1"/>
       <c r="U127" s="1"/>
+      <c r="V127" s="1"/>
+      <c r="W127" s="1"/>
+      <c r="X127" s="1"/>
+      <c r="Y127" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="128">
       <c r="A128" s="1"/>
@@ -3927,12 +4917,16 @@
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
       <c r="O128" s="1"/>
-      <c r="P128" s="1"/>
-      <c r="Q128" s="1"/>
+      <c r="P128" s="2"/>
+      <c r="Q128" s="2"/>
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
       <c r="T128" s="1"/>
       <c r="U128" s="1"/>
+      <c r="V128" s="1"/>
+      <c r="W128" s="1"/>
+      <c r="X128" s="1"/>
+      <c r="Y128" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="129">
       <c r="A129" s="1"/>
@@ -3950,12 +4944,16 @@
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
       <c r="O129" s="1"/>
-      <c r="P129" s="1"/>
-      <c r="Q129" s="1"/>
+      <c r="P129" s="2"/>
+      <c r="Q129" s="2"/>
       <c r="R129" s="1"/>
       <c r="S129" s="1"/>
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
+      <c r="V129" s="1"/>
+      <c r="W129" s="1"/>
+      <c r="X129" s="1"/>
+      <c r="Y129" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="130">
       <c r="A130" s="1"/>
@@ -3973,12 +4971,16 @@
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
       <c r="O130" s="1"/>
-      <c r="P130" s="1"/>
-      <c r="Q130" s="1"/>
+      <c r="P130" s="2"/>
+      <c r="Q130" s="2"/>
       <c r="R130" s="1"/>
       <c r="S130" s="1"/>
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
+      <c r="V130" s="1"/>
+      <c r="W130" s="1"/>
+      <c r="X130" s="1"/>
+      <c r="Y130" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="131">
       <c r="A131" s="1"/>
@@ -3996,12 +4998,16 @@
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
-      <c r="P131" s="1"/>
-      <c r="Q131" s="1"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
       <c r="R131" s="1"/>
       <c r="S131" s="1"/>
       <c r="T131" s="1"/>
       <c r="U131" s="1"/>
+      <c r="V131" s="1"/>
+      <c r="W131" s="1"/>
+      <c r="X131" s="1"/>
+      <c r="Y131" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="132">
       <c r="A132" s="1"/>
@@ -4019,12 +5025,16 @@
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
       <c r="O132" s="1"/>
-      <c r="P132" s="1"/>
-      <c r="Q132" s="1"/>
+      <c r="P132" s="2"/>
+      <c r="Q132" s="2"/>
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
+      <c r="V132" s="1"/>
+      <c r="W132" s="1"/>
+      <c r="X132" s="1"/>
+      <c r="Y132" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="133">
       <c r="A133" s="1"/>
@@ -4042,12 +5052,16 @@
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
       <c r="O133" s="1"/>
-      <c r="P133" s="1"/>
-      <c r="Q133" s="1"/>
+      <c r="P133" s="2"/>
+      <c r="Q133" s="2"/>
       <c r="R133" s="1"/>
       <c r="S133" s="1"/>
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
+      <c r="V133" s="1"/>
+      <c r="W133" s="1"/>
+      <c r="X133" s="1"/>
+      <c r="Y133" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="134">
       <c r="A134" s="1"/>
@@ -4065,12 +5079,16 @@
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
       <c r="O134" s="1"/>
-      <c r="P134" s="1"/>
-      <c r="Q134" s="1"/>
+      <c r="P134" s="2"/>
+      <c r="Q134" s="2"/>
       <c r="R134" s="1"/>
       <c r="S134" s="1"/>
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
+      <c r="V134" s="1"/>
+      <c r="W134" s="1"/>
+      <c r="X134" s="1"/>
+      <c r="Y134" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="135">
       <c r="A135" s="1"/>
@@ -4088,12 +5106,16 @@
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
-      <c r="P135" s="1"/>
-      <c r="Q135" s="1"/>
+      <c r="P135" s="2"/>
+      <c r="Q135" s="2"/>
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
       <c r="T135" s="1"/>
       <c r="U135" s="1"/>
+      <c r="V135" s="1"/>
+      <c r="W135" s="1"/>
+      <c r="X135" s="1"/>
+      <c r="Y135" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="136">
       <c r="A136" s="1"/>
@@ -4111,12 +5133,16 @@
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
       <c r="O136" s="1"/>
-      <c r="P136" s="1"/>
-      <c r="Q136" s="1"/>
+      <c r="P136" s="2"/>
+      <c r="Q136" s="2"/>
       <c r="R136" s="1"/>
       <c r="S136" s="1"/>
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
+      <c r="V136" s="1"/>
+      <c r="W136" s="1"/>
+      <c r="X136" s="1"/>
+      <c r="Y136" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="137">
       <c r="A137" s="1"/>
@@ -4134,12 +5160,16 @@
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
       <c r="O137" s="1"/>
-      <c r="P137" s="1"/>
-      <c r="Q137" s="1"/>
+      <c r="P137" s="2"/>
+      <c r="Q137" s="2"/>
       <c r="R137" s="1"/>
       <c r="S137" s="1"/>
       <c r="T137" s="1"/>
       <c r="U137" s="1"/>
+      <c r="V137" s="1"/>
+      <c r="W137" s="1"/>
+      <c r="X137" s="1"/>
+      <c r="Y137" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="138">
       <c r="A138" s="1"/>
@@ -4157,12 +5187,16 @@
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
       <c r="O138" s="1"/>
-      <c r="P138" s="1"/>
-      <c r="Q138" s="1"/>
+      <c r="P138" s="2"/>
+      <c r="Q138" s="2"/>
       <c r="R138" s="1"/>
       <c r="S138" s="1"/>
       <c r="T138" s="1"/>
       <c r="U138" s="1"/>
+      <c r="V138" s="1"/>
+      <c r="W138" s="1"/>
+      <c r="X138" s="1"/>
+      <c r="Y138" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="139">
       <c r="A139" s="1"/>
@@ -4180,12 +5214,16 @@
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
-      <c r="P139" s="1"/>
-      <c r="Q139" s="1"/>
+      <c r="P139" s="2"/>
+      <c r="Q139" s="2"/>
       <c r="R139" s="1"/>
       <c r="S139" s="1"/>
       <c r="T139" s="1"/>
       <c r="U139" s="1"/>
+      <c r="V139" s="1"/>
+      <c r="W139" s="1"/>
+      <c r="X139" s="1"/>
+      <c r="Y139" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="140">
       <c r="A140" s="1"/>
@@ -4203,12 +5241,16 @@
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
       <c r="O140" s="1"/>
-      <c r="P140" s="1"/>
-      <c r="Q140" s="1"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
       <c r="T140" s="1"/>
       <c r="U140" s="1"/>
+      <c r="V140" s="1"/>
+      <c r="W140" s="1"/>
+      <c r="X140" s="1"/>
+      <c r="Y140" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="141">
       <c r="A141" s="1"/>
@@ -4226,12 +5268,16 @@
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
       <c r="O141" s="1"/>
-      <c r="P141" s="1"/>
-      <c r="Q141" s="1"/>
+      <c r="P141" s="2"/>
+      <c r="Q141" s="2"/>
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
+      <c r="V141" s="1"/>
+      <c r="W141" s="1"/>
+      <c r="X141" s="1"/>
+      <c r="Y141" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="142">
       <c r="A142" s="1"/>
@@ -4249,12 +5295,16 @@
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
       <c r="O142" s="1"/>
-      <c r="P142" s="1"/>
-      <c r="Q142" s="1"/>
+      <c r="P142" s="2"/>
+      <c r="Q142" s="2"/>
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
       <c r="T142" s="1"/>
       <c r="U142" s="1"/>
+      <c r="V142" s="1"/>
+      <c r="W142" s="1"/>
+      <c r="X142" s="1"/>
+      <c r="Y142" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="143">
       <c r="A143" s="1"/>
@@ -4272,12 +5322,16 @@
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
-      <c r="P143" s="1"/>
-      <c r="Q143" s="1"/>
+      <c r="P143" s="2"/>
+      <c r="Q143" s="2"/>
       <c r="R143" s="1"/>
       <c r="S143" s="1"/>
       <c r="T143" s="1"/>
       <c r="U143" s="1"/>
+      <c r="V143" s="1"/>
+      <c r="W143" s="1"/>
+      <c r="X143" s="1"/>
+      <c r="Y143" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="144">
       <c r="A144" s="1"/>
@@ -4295,12 +5349,16 @@
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
       <c r="O144" s="1"/>
-      <c r="P144" s="1"/>
-      <c r="Q144" s="1"/>
+      <c r="P144" s="2"/>
+      <c r="Q144" s="2"/>
       <c r="R144" s="1"/>
       <c r="S144" s="1"/>
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
+      <c r="V144" s="1"/>
+      <c r="W144" s="1"/>
+      <c r="X144" s="1"/>
+      <c r="Y144" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="145">
       <c r="A145" s="1"/>
@@ -4318,12 +5376,16 @@
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
       <c r="O145" s="1"/>
-      <c r="P145" s="1"/>
-      <c r="Q145" s="1"/>
+      <c r="P145" s="2"/>
+      <c r="Q145" s="2"/>
       <c r="R145" s="1"/>
       <c r="S145" s="1"/>
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
+      <c r="V145" s="1"/>
+      <c r="W145" s="1"/>
+      <c r="X145" s="1"/>
+      <c r="Y145" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="146">
       <c r="A146" s="1"/>
@@ -4341,12 +5403,16 @@
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
       <c r="O146" s="1"/>
-      <c r="P146" s="1"/>
-      <c r="Q146" s="1"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
       <c r="T146" s="1"/>
       <c r="U146" s="1"/>
+      <c r="V146" s="1"/>
+      <c r="W146" s="1"/>
+      <c r="X146" s="1"/>
+      <c r="Y146" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="147">
       <c r="A147" s="1"/>
@@ -4364,12 +5430,16 @@
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>
-      <c r="P147" s="1"/>
-      <c r="Q147" s="1"/>
+      <c r="P147" s="2"/>
+      <c r="Q147" s="2"/>
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
       <c r="T147" s="1"/>
       <c r="U147" s="1"/>
+      <c r="V147" s="1"/>
+      <c r="W147" s="1"/>
+      <c r="X147" s="1"/>
+      <c r="Y147" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="148">
       <c r="A148" s="1"/>
@@ -4387,12 +5457,16 @@
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
       <c r="O148" s="1"/>
-      <c r="P148" s="1"/>
-      <c r="Q148" s="1"/>
+      <c r="P148" s="2"/>
+      <c r="Q148" s="2"/>
       <c r="R148" s="1"/>
       <c r="S148" s="1"/>
       <c r="T148" s="1"/>
       <c r="U148" s="1"/>
+      <c r="V148" s="1"/>
+      <c r="W148" s="1"/>
+      <c r="X148" s="1"/>
+      <c r="Y148" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="149">
       <c r="A149" s="1"/>
@@ -4410,12 +5484,16 @@
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
       <c r="O149" s="1"/>
-      <c r="P149" s="1"/>
-      <c r="Q149" s="1"/>
+      <c r="P149" s="2"/>
+      <c r="Q149" s="2"/>
       <c r="R149" s="1"/>
       <c r="S149" s="1"/>
       <c r="T149" s="1"/>
       <c r="U149" s="1"/>
+      <c r="V149" s="1"/>
+      <c r="W149" s="1"/>
+      <c r="X149" s="1"/>
+      <c r="Y149" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="150">
       <c r="A150" s="1"/>
@@ -4433,12 +5511,16 @@
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
       <c r="O150" s="1"/>
-      <c r="P150" s="1"/>
-      <c r="Q150" s="1"/>
+      <c r="P150" s="2"/>
+      <c r="Q150" s="2"/>
       <c r="R150" s="1"/>
       <c r="S150" s="1"/>
       <c r="T150" s="1"/>
       <c r="U150" s="1"/>
+      <c r="V150" s="1"/>
+      <c r="W150" s="1"/>
+      <c r="X150" s="1"/>
+      <c r="Y150" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="151">
       <c r="A151" s="1"/>
@@ -4456,12 +5538,16 @@
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
       <c r="O151" s="1"/>
-      <c r="P151" s="1"/>
-      <c r="Q151" s="1"/>
+      <c r="P151" s="2"/>
+      <c r="Q151" s="2"/>
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
       <c r="T151" s="1"/>
       <c r="U151" s="1"/>
+      <c r="V151" s="1"/>
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+      <c r="Y151" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="152">
       <c r="A152" s="1"/>
@@ -4479,12 +5565,16 @@
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
       <c r="O152" s="1"/>
-      <c r="P152" s="1"/>
-      <c r="Q152" s="1"/>
+      <c r="P152" s="2"/>
+      <c r="Q152" s="2"/>
       <c r="R152" s="1"/>
       <c r="S152" s="1"/>
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>
+      <c r="V152" s="1"/>
+      <c r="W152" s="1"/>
+      <c r="X152" s="1"/>
+      <c r="Y152" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="153">
       <c r="A153" s="1"/>
@@ -4502,12 +5592,16 @@
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
       <c r="O153" s="1"/>
-      <c r="P153" s="1"/>
-      <c r="Q153" s="1"/>
+      <c r="P153" s="2"/>
+      <c r="Q153" s="2"/>
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
       <c r="T153" s="1"/>
       <c r="U153" s="1"/>
+      <c r="V153" s="1"/>
+      <c r="W153" s="1"/>
+      <c r="X153" s="1"/>
+      <c r="Y153" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="154">
       <c r="A154" s="1"/>
@@ -4525,12 +5619,16 @@
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
       <c r="O154" s="1"/>
-      <c r="P154" s="1"/>
-      <c r="Q154" s="1"/>
+      <c r="P154" s="2"/>
+      <c r="Q154" s="2"/>
       <c r="R154" s="1"/>
       <c r="S154" s="1"/>
       <c r="T154" s="1"/>
       <c r="U154" s="1"/>
+      <c r="V154" s="1"/>
+      <c r="W154" s="1"/>
+      <c r="X154" s="1"/>
+      <c r="Y154" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="155">
       <c r="A155" s="1"/>
@@ -4548,12 +5646,16 @@
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
       <c r="O155" s="1"/>
-      <c r="P155" s="1"/>
-      <c r="Q155" s="1"/>
+      <c r="P155" s="2"/>
+      <c r="Q155" s="2"/>
       <c r="R155" s="1"/>
       <c r="S155" s="1"/>
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
+      <c r="V155" s="1"/>
+      <c r="W155" s="1"/>
+      <c r="X155" s="1"/>
+      <c r="Y155" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="156">
       <c r="A156" s="1"/>
@@ -4571,12 +5673,16 @@
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
       <c r="O156" s="1"/>
-      <c r="P156" s="1"/>
-      <c r="Q156" s="1"/>
+      <c r="P156" s="2"/>
+      <c r="Q156" s="2"/>
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
+      <c r="V156" s="1"/>
+      <c r="W156" s="1"/>
+      <c r="X156" s="1"/>
+      <c r="Y156" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="157">
       <c r="A157" s="1"/>
@@ -4594,12 +5700,16 @@
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
       <c r="O157" s="1"/>
-      <c r="P157" s="1"/>
-      <c r="Q157" s="1"/>
+      <c r="P157" s="2"/>
+      <c r="Q157" s="2"/>
       <c r="R157" s="1"/>
       <c r="S157" s="1"/>
       <c r="T157" s="1"/>
       <c r="U157" s="1"/>
+      <c r="V157" s="1"/>
+      <c r="W157" s="1"/>
+      <c r="X157" s="1"/>
+      <c r="Y157" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="158">
       <c r="A158" s="1"/>
@@ -4617,12 +5727,16 @@
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
       <c r="O158" s="1"/>
-      <c r="P158" s="1"/>
-      <c r="Q158" s="1"/>
+      <c r="P158" s="2"/>
+      <c r="Q158" s="2"/>
       <c r="R158" s="1"/>
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
       <c r="U158" s="1"/>
+      <c r="V158" s="1"/>
+      <c r="W158" s="1"/>
+      <c r="X158" s="1"/>
+      <c r="Y158" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="159">
       <c r="A159" s="1"/>
@@ -4640,12 +5754,16 @@
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
       <c r="O159" s="1"/>
-      <c r="P159" s="1"/>
-      <c r="Q159" s="1"/>
+      <c r="P159" s="2"/>
+      <c r="Q159" s="2"/>
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
+      <c r="V159" s="1"/>
+      <c r="W159" s="1"/>
+      <c r="X159" s="1"/>
+      <c r="Y159" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="160">
       <c r="A160" s="1"/>
@@ -4663,12 +5781,16 @@
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
       <c r="O160" s="1"/>
-      <c r="P160" s="1"/>
-      <c r="Q160" s="1"/>
+      <c r="P160" s="2"/>
+      <c r="Q160" s="2"/>
       <c r="R160" s="1"/>
       <c r="S160" s="1"/>
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
+      <c r="V160" s="1"/>
+      <c r="W160" s="1"/>
+      <c r="X160" s="1"/>
+      <c r="Y160" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="161">
       <c r="A161" s="1"/>
@@ -4686,12 +5808,16 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
       <c r="O161" s="1"/>
-      <c r="P161" s="1"/>
-      <c r="Q161" s="1"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
       <c r="R161" s="1"/>
       <c r="S161" s="1"/>
       <c r="T161" s="1"/>
       <c r="U161" s="1"/>
+      <c r="V161" s="1"/>
+      <c r="W161" s="1"/>
+      <c r="X161" s="1"/>
+      <c r="Y161" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="162">
       <c r="A162" s="1"/>
@@ -4709,12 +5835,16 @@
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
       <c r="O162" s="1"/>
-      <c r="P162" s="1"/>
-      <c r="Q162" s="1"/>
+      <c r="P162" s="2"/>
+      <c r="Q162" s="2"/>
       <c r="R162" s="1"/>
       <c r="S162" s="1"/>
       <c r="T162" s="1"/>
       <c r="U162" s="1"/>
+      <c r="V162" s="1"/>
+      <c r="W162" s="1"/>
+      <c r="X162" s="1"/>
+      <c r="Y162" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="163">
       <c r="A163" s="1"/>
@@ -4732,12 +5862,16 @@
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
       <c r="O163" s="1"/>
-      <c r="P163" s="1"/>
-      <c r="Q163" s="1"/>
+      <c r="P163" s="2"/>
+      <c r="Q163" s="2"/>
       <c r="R163" s="1"/>
       <c r="S163" s="1"/>
       <c r="T163" s="1"/>
       <c r="U163" s="1"/>
+      <c r="V163" s="1"/>
+      <c r="W163" s="1"/>
+      <c r="X163" s="1"/>
+      <c r="Y163" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="164">
       <c r="A164" s="1"/>
@@ -4755,12 +5889,16 @@
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
       <c r="O164" s="1"/>
-      <c r="P164" s="1"/>
-      <c r="Q164" s="1"/>
+      <c r="P164" s="2"/>
+      <c r="Q164" s="2"/>
       <c r="R164" s="1"/>
       <c r="S164" s="1"/>
       <c r="T164" s="1"/>
       <c r="U164" s="1"/>
+      <c r="V164" s="1"/>
+      <c r="W164" s="1"/>
+      <c r="X164" s="1"/>
+      <c r="Y164" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="165">
       <c r="A165" s="1"/>
@@ -4778,12 +5916,16 @@
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
       <c r="O165" s="1"/>
-      <c r="P165" s="1"/>
-      <c r="Q165" s="1"/>
+      <c r="P165" s="2"/>
+      <c r="Q165" s="2"/>
       <c r="R165" s="1"/>
       <c r="S165" s="1"/>
       <c r="T165" s="1"/>
       <c r="U165" s="1"/>
+      <c r="V165" s="1"/>
+      <c r="W165" s="1"/>
+      <c r="X165" s="1"/>
+      <c r="Y165" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="166">
       <c r="A166" s="1"/>
@@ -4801,12 +5943,16 @@
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
       <c r="O166" s="1"/>
-      <c r="P166" s="1"/>
-      <c r="Q166" s="1"/>
+      <c r="P166" s="2"/>
+      <c r="Q166" s="2"/>
       <c r="R166" s="1"/>
       <c r="S166" s="1"/>
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
+      <c r="V166" s="1"/>
+      <c r="W166" s="1"/>
+      <c r="X166" s="1"/>
+      <c r="Y166" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="167">
       <c r="A167" s="1"/>
@@ -4824,12 +5970,16 @@
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
       <c r="O167" s="1"/>
-      <c r="P167" s="1"/>
-      <c r="Q167" s="1"/>
+      <c r="P167" s="2"/>
+      <c r="Q167" s="2"/>
       <c r="R167" s="1"/>
       <c r="S167" s="1"/>
       <c r="T167" s="1"/>
       <c r="U167" s="1"/>
+      <c r="V167" s="1"/>
+      <c r="W167" s="1"/>
+      <c r="X167" s="1"/>
+      <c r="Y167" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="168">
       <c r="A168" s="1"/>
@@ -4847,12 +5997,16 @@
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
       <c r="O168" s="1"/>
-      <c r="P168" s="1"/>
-      <c r="Q168" s="1"/>
+      <c r="P168" s="2"/>
+      <c r="Q168" s="2"/>
       <c r="R168" s="1"/>
       <c r="S168" s="1"/>
       <c r="T168" s="1"/>
       <c r="U168" s="1"/>
+      <c r="V168" s="1"/>
+      <c r="W168" s="1"/>
+      <c r="X168" s="1"/>
+      <c r="Y168" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="169">
       <c r="A169" s="1"/>
@@ -4870,12 +6024,16 @@
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
       <c r="O169" s="1"/>
-      <c r="P169" s="1"/>
-      <c r="Q169" s="1"/>
+      <c r="P169" s="2"/>
+      <c r="Q169" s="2"/>
       <c r="R169" s="1"/>
       <c r="S169" s="1"/>
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
+      <c r="V169" s="1"/>
+      <c r="W169" s="1"/>
+      <c r="X169" s="1"/>
+      <c r="Y169" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="170">
       <c r="A170" s="1"/>
@@ -4893,12 +6051,16 @@
       <c r="M170" s="1"/>
       <c r="N170" s="1"/>
       <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-      <c r="Q170" s="1"/>
+      <c r="P170" s="2"/>
+      <c r="Q170" s="2"/>
       <c r="R170" s="1"/>
       <c r="S170" s="1"/>
       <c r="T170" s="1"/>
       <c r="U170" s="1"/>
+      <c r="V170" s="1"/>
+      <c r="W170" s="1"/>
+      <c r="X170" s="1"/>
+      <c r="Y170" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="171">
       <c r="A171" s="1"/>
@@ -4916,12 +6078,16 @@
       <c r="M171" s="1"/>
       <c r="N171" s="1"/>
       <c r="O171" s="1"/>
-      <c r="P171" s="1"/>
-      <c r="Q171" s="1"/>
+      <c r="P171" s="2"/>
+      <c r="Q171" s="2"/>
       <c r="R171" s="1"/>
       <c r="S171" s="1"/>
       <c r="T171" s="1"/>
       <c r="U171" s="1"/>
+      <c r="V171" s="1"/>
+      <c r="W171" s="1"/>
+      <c r="X171" s="1"/>
+      <c r="Y171" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="172">
       <c r="A172" s="1"/>
@@ -4939,12 +6105,16 @@
       <c r="M172" s="1"/>
       <c r="N172" s="1"/>
       <c r="O172" s="1"/>
-      <c r="P172" s="1"/>
-      <c r="Q172" s="1"/>
+      <c r="P172" s="2"/>
+      <c r="Q172" s="2"/>
       <c r="R172" s="1"/>
       <c r="S172" s="1"/>
       <c r="T172" s="1"/>
       <c r="U172" s="1"/>
+      <c r="V172" s="1"/>
+      <c r="W172" s="1"/>
+      <c r="X172" s="1"/>
+      <c r="Y172" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="173">
       <c r="A173" s="1"/>
@@ -4962,12 +6132,16 @@
       <c r="M173" s="1"/>
       <c r="N173" s="1"/>
       <c r="O173" s="1"/>
-      <c r="P173" s="1"/>
-      <c r="Q173" s="1"/>
+      <c r="P173" s="2"/>
+      <c r="Q173" s="2"/>
       <c r="R173" s="1"/>
       <c r="S173" s="1"/>
       <c r="T173" s="1"/>
       <c r="U173" s="1"/>
+      <c r="V173" s="1"/>
+      <c r="W173" s="1"/>
+      <c r="X173" s="1"/>
+      <c r="Y173" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="174">
       <c r="A174" s="1"/>
@@ -4985,12 +6159,16 @@
       <c r="M174" s="1"/>
       <c r="N174" s="1"/>
       <c r="O174" s="1"/>
-      <c r="P174" s="1"/>
-      <c r="Q174" s="1"/>
+      <c r="P174" s="2"/>
+      <c r="Q174" s="2"/>
       <c r="R174" s="1"/>
       <c r="S174" s="1"/>
       <c r="T174" s="1"/>
       <c r="U174" s="1"/>
+      <c r="V174" s="1"/>
+      <c r="W174" s="1"/>
+      <c r="X174" s="1"/>
+      <c r="Y174" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="175">
       <c r="A175" s="1"/>
@@ -5008,12 +6186,16 @@
       <c r="M175" s="1"/>
       <c r="N175" s="1"/>
       <c r="O175" s="1"/>
-      <c r="P175" s="1"/>
-      <c r="Q175" s="1"/>
+      <c r="P175" s="2"/>
+      <c r="Q175" s="2"/>
       <c r="R175" s="1"/>
       <c r="S175" s="1"/>
       <c r="T175" s="1"/>
       <c r="U175" s="1"/>
+      <c r="V175" s="1"/>
+      <c r="W175" s="1"/>
+      <c r="X175" s="1"/>
+      <c r="Y175" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="176">
       <c r="A176" s="1"/>
@@ -5031,12 +6213,16 @@
       <c r="M176" s="1"/>
       <c r="N176" s="1"/>
       <c r="O176" s="1"/>
-      <c r="P176" s="1"/>
-      <c r="Q176" s="1"/>
+      <c r="P176" s="2"/>
+      <c r="Q176" s="2"/>
       <c r="R176" s="1"/>
       <c r="S176" s="1"/>
       <c r="T176" s="1"/>
       <c r="U176" s="1"/>
+      <c r="V176" s="1"/>
+      <c r="W176" s="1"/>
+      <c r="X176" s="1"/>
+      <c r="Y176" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="177">
       <c r="A177" s="1"/>
@@ -5054,12 +6240,16 @@
       <c r="M177" s="1"/>
       <c r="N177" s="1"/>
       <c r="O177" s="1"/>
-      <c r="P177" s="1"/>
-      <c r="Q177" s="1"/>
+      <c r="P177" s="2"/>
+      <c r="Q177" s="2"/>
       <c r="R177" s="1"/>
       <c r="S177" s="1"/>
       <c r="T177" s="1"/>
       <c r="U177" s="1"/>
+      <c r="V177" s="1"/>
+      <c r="W177" s="1"/>
+      <c r="X177" s="1"/>
+      <c r="Y177" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="178">
       <c r="A178" s="1"/>
@@ -5077,12 +6267,16 @@
       <c r="M178" s="1"/>
       <c r="N178" s="1"/>
       <c r="O178" s="1"/>
-      <c r="P178" s="1"/>
-      <c r="Q178" s="1"/>
+      <c r="P178" s="2"/>
+      <c r="Q178" s="2"/>
       <c r="R178" s="1"/>
       <c r="S178" s="1"/>
       <c r="T178" s="1"/>
       <c r="U178" s="1"/>
+      <c r="V178" s="1"/>
+      <c r="W178" s="1"/>
+      <c r="X178" s="1"/>
+      <c r="Y178" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="179">
       <c r="A179" s="1"/>
@@ -5100,12 +6294,16 @@
       <c r="M179" s="1"/>
       <c r="N179" s="1"/>
       <c r="O179" s="1"/>
-      <c r="P179" s="1"/>
-      <c r="Q179" s="1"/>
+      <c r="P179" s="2"/>
+      <c r="Q179" s="2"/>
       <c r="R179" s="1"/>
       <c r="S179" s="1"/>
       <c r="T179" s="1"/>
       <c r="U179" s="1"/>
+      <c r="V179" s="1"/>
+      <c r="W179" s="1"/>
+      <c r="X179" s="1"/>
+      <c r="Y179" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="180">
       <c r="A180" s="1"/>
@@ -5123,12 +6321,16 @@
       <c r="M180" s="1"/>
       <c r="N180" s="1"/>
       <c r="O180" s="1"/>
-      <c r="P180" s="1"/>
-      <c r="Q180" s="1"/>
+      <c r="P180" s="2"/>
+      <c r="Q180" s="2"/>
       <c r="R180" s="1"/>
       <c r="S180" s="1"/>
       <c r="T180" s="1"/>
       <c r="U180" s="1"/>
+      <c r="V180" s="1"/>
+      <c r="W180" s="1"/>
+      <c r="X180" s="1"/>
+      <c r="Y180" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="181">
       <c r="A181" s="1"/>
@@ -5146,12 +6348,16 @@
       <c r="M181" s="1"/>
       <c r="N181" s="1"/>
       <c r="O181" s="1"/>
-      <c r="P181" s="1"/>
-      <c r="Q181" s="1"/>
+      <c r="P181" s="2"/>
+      <c r="Q181" s="2"/>
       <c r="R181" s="1"/>
       <c r="S181" s="1"/>
       <c r="T181" s="1"/>
       <c r="U181" s="1"/>
+      <c r="V181" s="1"/>
+      <c r="W181" s="1"/>
+      <c r="X181" s="1"/>
+      <c r="Y181" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="182">
       <c r="A182" s="1"/>
@@ -5169,12 +6375,16 @@
       <c r="M182" s="1"/>
       <c r="N182" s="1"/>
       <c r="O182" s="1"/>
-      <c r="P182" s="1"/>
-      <c r="Q182" s="1"/>
+      <c r="P182" s="2"/>
+      <c r="Q182" s="2"/>
       <c r="R182" s="1"/>
       <c r="S182" s="1"/>
       <c r="T182" s="1"/>
       <c r="U182" s="1"/>
+      <c r="V182" s="1"/>
+      <c r="W182" s="1"/>
+      <c r="X182" s="1"/>
+      <c r="Y182" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="183">
       <c r="A183" s="1"/>
@@ -5192,12 +6402,16 @@
       <c r="M183" s="1"/>
       <c r="N183" s="1"/>
       <c r="O183" s="1"/>
-      <c r="P183" s="1"/>
-      <c r="Q183" s="1"/>
+      <c r="P183" s="2"/>
+      <c r="Q183" s="2"/>
       <c r="R183" s="1"/>
       <c r="S183" s="1"/>
       <c r="T183" s="1"/>
       <c r="U183" s="1"/>
+      <c r="V183" s="1"/>
+      <c r="W183" s="1"/>
+      <c r="X183" s="1"/>
+      <c r="Y183" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="184">
       <c r="A184" s="1"/>
@@ -5215,12 +6429,16 @@
       <c r="M184" s="1"/>
       <c r="N184" s="1"/>
       <c r="O184" s="1"/>
-      <c r="P184" s="1"/>
-      <c r="Q184" s="1"/>
+      <c r="P184" s="2"/>
+      <c r="Q184" s="2"/>
       <c r="R184" s="1"/>
       <c r="S184" s="1"/>
       <c r="T184" s="1"/>
       <c r="U184" s="1"/>
+      <c r="V184" s="1"/>
+      <c r="W184" s="1"/>
+      <c r="X184" s="1"/>
+      <c r="Y184" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="185">
       <c r="A185" s="1"/>
@@ -5238,12 +6456,16 @@
       <c r="M185" s="1"/>
       <c r="N185" s="1"/>
       <c r="O185" s="1"/>
-      <c r="P185" s="1"/>
-      <c r="Q185" s="1"/>
+      <c r="P185" s="2"/>
+      <c r="Q185" s="2"/>
       <c r="R185" s="1"/>
       <c r="S185" s="1"/>
       <c r="T185" s="1"/>
       <c r="U185" s="1"/>
+      <c r="V185" s="1"/>
+      <c r="W185" s="1"/>
+      <c r="X185" s="1"/>
+      <c r="Y185" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="186">
       <c r="A186" s="1"/>
@@ -5261,12 +6483,16 @@
       <c r="M186" s="1"/>
       <c r="N186" s="1"/>
       <c r="O186" s="1"/>
-      <c r="P186" s="1"/>
-      <c r="Q186" s="1"/>
+      <c r="P186" s="2"/>
+      <c r="Q186" s="2"/>
       <c r="R186" s="1"/>
       <c r="S186" s="1"/>
       <c r="T186" s="1"/>
       <c r="U186" s="1"/>
+      <c r="V186" s="1"/>
+      <c r="W186" s="1"/>
+      <c r="X186" s="1"/>
+      <c r="Y186" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="187">
       <c r="A187" s="1"/>
@@ -5284,12 +6510,16 @@
       <c r="M187" s="1"/>
       <c r="N187" s="1"/>
       <c r="O187" s="1"/>
-      <c r="P187" s="1"/>
-      <c r="Q187" s="1"/>
+      <c r="P187" s="2"/>
+      <c r="Q187" s="2"/>
       <c r="R187" s="1"/>
       <c r="S187" s="1"/>
       <c r="T187" s="1"/>
       <c r="U187" s="1"/>
+      <c r="V187" s="1"/>
+      <c r="W187" s="1"/>
+      <c r="X187" s="1"/>
+      <c r="Y187" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="188">
       <c r="A188" s="1"/>
@@ -5307,12 +6537,16 @@
       <c r="M188" s="1"/>
       <c r="N188" s="1"/>
       <c r="O188" s="1"/>
-      <c r="P188" s="1"/>
-      <c r="Q188" s="1"/>
+      <c r="P188" s="2"/>
+      <c r="Q188" s="2"/>
       <c r="R188" s="1"/>
       <c r="S188" s="1"/>
       <c r="T188" s="1"/>
       <c r="U188" s="1"/>
+      <c r="V188" s="1"/>
+      <c r="W188" s="1"/>
+      <c r="X188" s="1"/>
+      <c r="Y188" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="189">
       <c r="A189" s="1"/>
@@ -5330,12 +6564,16 @@
       <c r="M189" s="1"/>
       <c r="N189" s="1"/>
       <c r="O189" s="1"/>
-      <c r="P189" s="1"/>
-      <c r="Q189" s="1"/>
+      <c r="P189" s="2"/>
+      <c r="Q189" s="2"/>
       <c r="R189" s="1"/>
       <c r="S189" s="1"/>
       <c r="T189" s="1"/>
       <c r="U189" s="1"/>
+      <c r="V189" s="1"/>
+      <c r="W189" s="1"/>
+      <c r="X189" s="1"/>
+      <c r="Y189" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="190">
       <c r="A190" s="1"/>
@@ -5353,12 +6591,16 @@
       <c r="M190" s="1"/>
       <c r="N190" s="1"/>
       <c r="O190" s="1"/>
-      <c r="P190" s="1"/>
-      <c r="Q190" s="1"/>
+      <c r="P190" s="2"/>
+      <c r="Q190" s="2"/>
       <c r="R190" s="1"/>
       <c r="S190" s="1"/>
       <c r="T190" s="1"/>
       <c r="U190" s="1"/>
+      <c r="V190" s="1"/>
+      <c r="W190" s="1"/>
+      <c r="X190" s="1"/>
+      <c r="Y190" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="191">
       <c r="A191" s="1"/>
@@ -5376,12 +6618,16 @@
       <c r="M191" s="1"/>
       <c r="N191" s="1"/>
       <c r="O191" s="1"/>
-      <c r="P191" s="1"/>
-      <c r="Q191" s="1"/>
+      <c r="P191" s="2"/>
+      <c r="Q191" s="2"/>
       <c r="R191" s="1"/>
       <c r="S191" s="1"/>
       <c r="T191" s="1"/>
       <c r="U191" s="1"/>
+      <c r="V191" s="1"/>
+      <c r="W191" s="1"/>
+      <c r="X191" s="1"/>
+      <c r="Y191" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="192">
       <c r="A192" s="1"/>
@@ -5399,12 +6645,16 @@
       <c r="M192" s="1"/>
       <c r="N192" s="1"/>
       <c r="O192" s="1"/>
-      <c r="P192" s="1"/>
-      <c r="Q192" s="1"/>
+      <c r="P192" s="2"/>
+      <c r="Q192" s="2"/>
       <c r="R192" s="1"/>
       <c r="S192" s="1"/>
       <c r="T192" s="1"/>
       <c r="U192" s="1"/>
+      <c r="V192" s="1"/>
+      <c r="W192" s="1"/>
+      <c r="X192" s="1"/>
+      <c r="Y192" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="193">
       <c r="A193" s="1"/>
@@ -5422,12 +6672,16 @@
       <c r="M193" s="1"/>
       <c r="N193" s="1"/>
       <c r="O193" s="1"/>
-      <c r="P193" s="1"/>
-      <c r="Q193" s="1"/>
+      <c r="P193" s="2"/>
+      <c r="Q193" s="2"/>
       <c r="R193" s="1"/>
       <c r="S193" s="1"/>
       <c r="T193" s="1"/>
       <c r="U193" s="1"/>
+      <c r="V193" s="1"/>
+      <c r="W193" s="1"/>
+      <c r="X193" s="1"/>
+      <c r="Y193" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="194">
       <c r="A194" s="1"/>
@@ -5445,12 +6699,16 @@
       <c r="M194" s="1"/>
       <c r="N194" s="1"/>
       <c r="O194" s="1"/>
-      <c r="P194" s="1"/>
-      <c r="Q194" s="1"/>
+      <c r="P194" s="2"/>
+      <c r="Q194" s="2"/>
       <c r="R194" s="1"/>
       <c r="S194" s="1"/>
       <c r="T194" s="1"/>
       <c r="U194" s="1"/>
+      <c r="V194" s="1"/>
+      <c r="W194" s="1"/>
+      <c r="X194" s="1"/>
+      <c r="Y194" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="195">
       <c r="A195" s="1"/>
@@ -5468,12 +6726,16 @@
       <c r="M195" s="1"/>
       <c r="N195" s="1"/>
       <c r="O195" s="1"/>
-      <c r="P195" s="1"/>
-      <c r="Q195" s="1"/>
+      <c r="P195" s="2"/>
+      <c r="Q195" s="2"/>
       <c r="R195" s="1"/>
       <c r="S195" s="1"/>
       <c r="T195" s="1"/>
       <c r="U195" s="1"/>
+      <c r="V195" s="1"/>
+      <c r="W195" s="1"/>
+      <c r="X195" s="1"/>
+      <c r="Y195" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="196">
       <c r="A196" s="1"/>
@@ -5491,12 +6753,16 @@
       <c r="M196" s="1"/>
       <c r="N196" s="1"/>
       <c r="O196" s="1"/>
-      <c r="P196" s="1"/>
-      <c r="Q196" s="1"/>
+      <c r="P196" s="2"/>
+      <c r="Q196" s="2"/>
       <c r="R196" s="1"/>
       <c r="S196" s="1"/>
       <c r="T196" s="1"/>
       <c r="U196" s="1"/>
+      <c r="V196" s="1"/>
+      <c r="W196" s="1"/>
+      <c r="X196" s="1"/>
+      <c r="Y196" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="197">
       <c r="A197" s="1"/>
@@ -5514,12 +6780,16 @@
       <c r="M197" s="1"/>
       <c r="N197" s="1"/>
       <c r="O197" s="1"/>
-      <c r="P197" s="1"/>
-      <c r="Q197" s="1"/>
+      <c r="P197" s="2"/>
+      <c r="Q197" s="2"/>
       <c r="R197" s="1"/>
       <c r="S197" s="1"/>
       <c r="T197" s="1"/>
       <c r="U197" s="1"/>
+      <c r="V197" s="1"/>
+      <c r="W197" s="1"/>
+      <c r="X197" s="1"/>
+      <c r="Y197" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="198">
       <c r="A198" s="1"/>
@@ -5537,12 +6807,16 @@
       <c r="M198" s="1"/>
       <c r="N198" s="1"/>
       <c r="O198" s="1"/>
-      <c r="P198" s="1"/>
-      <c r="Q198" s="1"/>
+      <c r="P198" s="2"/>
+      <c r="Q198" s="2"/>
       <c r="R198" s="1"/>
       <c r="S198" s="1"/>
       <c r="T198" s="1"/>
       <c r="U198" s="1"/>
+      <c r="V198" s="1"/>
+      <c r="W198" s="1"/>
+      <c r="X198" s="1"/>
+      <c r="Y198" s="1"/>
     </row>
     <row customHeight="true" ht="113" r="199">
       <c r="A199" s="1"/>
@@ -5560,37 +6834,19 @@
       <c r="M199" s="1"/>
       <c r="N199" s="1"/>
       <c r="O199" s="1"/>
-      <c r="P199" s="1"/>
-      <c r="Q199" s="1"/>
+      <c r="P199" s="2"/>
+      <c r="Q199" s="2"/>
       <c r="R199" s="1"/>
       <c r="S199" s="1"/>
       <c r="T199" s="1"/>
       <c r="U199" s="1"/>
-    </row>
-    <row customHeight="true" ht="113" r="200">
-      <c r="A200" s="1"/>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1"/>
-      <c r="E200" s="1"/>
-      <c r="F200" s="1"/>
-      <c r="G200" s="1"/>
-      <c r="H200" s="1"/>
-      <c r="I200" s="1"/>
-      <c r="J200" s="1"/>
-      <c r="K200" s="1"/>
-      <c r="L200" s="1"/>
-      <c r="M200" s="1"/>
-      <c r="N200" s="1"/>
-      <c r="O200" s="1"/>
-      <c r="P200" s="1"/>
-      <c r="Q200" s="1"/>
-      <c r="R200" s="1"/>
-      <c r="S200" s="1"/>
-      <c r="T200" s="1"/>
-      <c r="U200" s="1"/>
+      <c r="V199" s="1"/>
+      <c r="W199" s="1"/>
+      <c r="X199" s="1"/>
+      <c r="Y199" s="1"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>